<commit_message>
raccolti dati piano inclinato
</commit_message>
<xml_diff>
--- a/URTI/urti_dati.xlsx
+++ b/URTI/urti_dati.xlsx
@@ -116,9 +116,13 @@
   <cellStyleXfs count="1">
     <xf fontId="0" fillId="0" borderId="0" numFmtId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="5">
     <xf fontId="0" fillId="0" borderId="0" numFmtId="0" xfId="0"/>
     <xf fontId="0" fillId="0" borderId="0" numFmtId="160" xfId="0" applyNumberFormat="1"/>
+    <xf fontId="0" fillId="0" borderId="0" numFmtId="161" xfId="0" applyNumberFormat="1"/>
+    <xf fontId="0" fillId="0" borderId="0" numFmtId="0" xfId="0">
+      <protection hidden="0" locked="1"/>
+    </xf>
     <xf fontId="0" fillId="0" borderId="0" numFmtId="161" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
@@ -1045,8 +1049,12 @@
       <c r="B2">
         <v>0.00080000000000000004</v>
       </c>
-      <c r="C2" s="1"/>
-      <c r="D2" s="2"/>
+      <c r="C2" s="1">
+        <v>0.39300000000000002</v>
+      </c>
+      <c r="D2" s="2">
+        <v>0.0012999999999999999</v>
+      </c>
       <c r="E2">
         <v>10</v>
       </c>
@@ -1064,8 +1072,12 @@
       <c r="B3">
         <v>0.00059999999999999995</v>
       </c>
-      <c r="C3" s="1"/>
-      <c r="D3" s="2"/>
+      <c r="C3" s="1">
+        <v>0.39400000000000002</v>
+      </c>
+      <c r="D3" s="2">
+        <v>0.0012999999999999999</v>
+      </c>
     </row>
     <row r="4" ht="14.25">
       <c r="A4">
@@ -1074,8 +1086,12 @@
       <c r="B4">
         <v>0.00089999999999999998</v>
       </c>
-      <c r="C4" s="1"/>
-      <c r="D4" s="2"/>
+      <c r="C4" s="1">
+        <v>0.38900000000000001</v>
+      </c>
+      <c r="D4" s="2">
+        <v>0.0011000000000000001</v>
+      </c>
     </row>
     <row r="5" ht="14.25">
       <c r="A5">
@@ -1084,8 +1100,12 @@
       <c r="B5">
         <v>0.00069999999999999999</v>
       </c>
-      <c r="C5" s="1"/>
-      <c r="D5" s="2"/>
+      <c r="C5" s="1">
+        <v>0.38800000000000001</v>
+      </c>
+      <c r="D5" s="2">
+        <v>0.0014</v>
+      </c>
     </row>
     <row r="6" ht="14.25">
       <c r="A6">
@@ -1094,8 +1114,12 @@
       <c r="B6">
         <v>0.00069999999999999999</v>
       </c>
-      <c r="C6" s="1"/>
-      <c r="D6" s="2"/>
+      <c r="C6" s="1">
+        <v>0.38500000000000001</v>
+      </c>
+      <c r="D6" s="2">
+        <v>0.0011999999999999999</v>
+      </c>
     </row>
     <row r="7" ht="14.25">
       <c r="A7">
@@ -1104,8 +1128,12 @@
       <c r="B7">
         <v>0.00069999999999999999</v>
       </c>
-      <c r="C7" s="1"/>
-      <c r="D7" s="2"/>
+      <c r="C7" s="1">
+        <v>0.38500000000000001</v>
+      </c>
+      <c r="D7" s="2">
+        <v>0.001</v>
+      </c>
     </row>
     <row r="8" ht="14.25">
       <c r="A8">
@@ -1114,8 +1142,12 @@
       <c r="B8">
         <v>0.00059999999999999995</v>
       </c>
-      <c r="C8" s="1"/>
-      <c r="D8" s="2"/>
+      <c r="C8" s="3">
+        <v>0.38500000000000001</v>
+      </c>
+      <c r="D8" s="3">
+        <v>0.00059999999999999995</v>
+      </c>
     </row>
     <row r="9" ht="14.25">
       <c r="A9">
@@ -1124,8 +1156,12 @@
       <c r="B9">
         <v>0.00069999999999999999</v>
       </c>
-      <c r="C9" s="1"/>
-      <c r="D9" s="2"/>
+      <c r="C9" s="3">
+        <v>0.38400000000000001</v>
+      </c>
+      <c r="D9" s="3">
+        <v>0.00080000000000000004</v>
+      </c>
     </row>
     <row r="10" ht="14.25">
       <c r="A10">
@@ -1134,8 +1170,12 @@
       <c r="B10">
         <v>0.00069999999999999999</v>
       </c>
-      <c r="C10" s="1"/>
-      <c r="D10" s="2"/>
+      <c r="C10" s="1">
+        <v>0.39900000000000002</v>
+      </c>
+      <c r="D10" s="2">
+        <v>0.00080000000000000004</v>
+      </c>
     </row>
     <row r="11" ht="14.25">
       <c r="A11">
@@ -1144,8 +1184,12 @@
       <c r="B11">
         <v>0.00050000000000000001</v>
       </c>
-      <c r="C11" s="1"/>
-      <c r="D11" s="2"/>
+      <c r="C11" s="1">
+        <v>0.38700000000000001</v>
+      </c>
+      <c r="D11" s="4">
+        <v>0.00089999999999999998</v>
+      </c>
     </row>
     <row r="12" ht="14.25">
       <c r="A12">
@@ -1154,9 +1198,15 @@
       <c r="B12">
         <v>0.0016999999999999999</v>
       </c>
-      <c r="C12" s="1"/>
-      <c r="D12" s="2"/>
-    </row>
+      <c r="C12" s="1">
+        <v>0.38500000000000001</v>
+      </c>
+      <c r="D12" s="2">
+        <v>0.00080000000000000004</v>
+      </c>
+    </row>
+    <row r="13" ht="14.25"/>
+    <row r="14" ht="14.25"/>
   </sheetData>
   <printOptions headings="0" gridLines="0"/>
   <pageMargins left="0.70078740157480324" right="0.70078740157480324" top="0.75196850393700787" bottom="0.75196850393700787" header="0.29999999999999999" footer="0.29999999999999999"/>

</xml_diff>

<commit_message>
urto anaelastico con pesi
</commit_message>
<xml_diff>
--- a/URTI/urti_dati.xlsx
+++ b/URTI/urti_dati.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <workbookPr/>
   <bookViews>
-    <workbookView xWindow="360" yWindow="15" windowWidth="20955" windowHeight="9720" activeTab="6"/>
+    <workbookView xWindow="360" yWindow="15" windowWidth="20955" windowHeight="9720" activeTab="8"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" state="visible" r:id="rId1"/>
@@ -13,13 +13,15 @@
     <sheet name="urto-magnete" sheetId="5" state="visible" r:id="rId5"/>
     <sheet name="urti-elastici" sheetId="6" state="visible" r:id="rId6"/>
     <sheet name="urti-anaelastici" sheetId="7" state="visible" r:id="rId7"/>
+    <sheet name="urto-anaelastico+massa" sheetId="8" state="visible" r:id="rId8"/>
+    <sheet name="urto-elastico+massa" sheetId="9" state="visible" r:id="rId9"/>
   </sheets>
   <calcPr/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="39" uniqueCount="39">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="43" uniqueCount="43">
   <si>
     <t xml:space="preserve">massa carrello blu</t>
   </si>
@@ -123,6 +125,12 @@
     <t>m_blu</t>
   </si>
   <si>
+    <t>Pi</t>
+  </si>
+  <si>
+    <t>Pf</t>
+  </si>
+  <si>
     <t>ViB</t>
   </si>
   <si>
@@ -136,6 +144,12 @@
   </si>
   <si>
     <t>ViR</t>
+  </si>
+  <si>
+    <t>deltaV</t>
+  </si>
+  <si>
+    <t>deltaV/Vi</t>
   </si>
 </sst>
 </file>
@@ -163,7 +177,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="1">
+  <borders count="2">
     <border>
       <left/>
       <right/>
@@ -171,11 +185,26 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color auto="1"/>
+      </left>
+      <right style="thin">
+        <color auto="1"/>
+      </right>
+      <top style="thin">
+        <color auto="1"/>
+      </top>
+      <bottom style="thin">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf fontId="0" fillId="0" borderId="0" numFmtId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
   </cellStyleXfs>
-  <cellXfs count="8">
+  <cellXfs count="9">
     <xf fontId="0" fillId="0" borderId="0" numFmtId="0" xfId="0"/>
     <xf fontId="0" fillId="0" borderId="0" numFmtId="160" xfId="0" applyNumberFormat="1"/>
     <xf fontId="0" fillId="0" borderId="0" numFmtId="161" xfId="0" applyNumberFormat="1"/>
@@ -186,6 +215,7 @@
     <xf fontId="0" fillId="0" borderId="0" numFmtId="2" xfId="0" applyNumberFormat="1"/>
     <xf fontId="0" fillId="0" borderId="0" numFmtId="162" xfId="0" applyNumberFormat="1"/>
     <xf fontId="0" fillId="0" borderId="0" numFmtId="0" xfId="0"/>
+    <xf fontId="0" fillId="0" borderId="1" numFmtId="2" xfId="0" applyNumberFormat="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1831,10 +1861,28 @@
       <c r="D1" t="s">
         <v>33</v>
       </c>
+      <c r="E1" t="s">
+        <v>25</v>
+      </c>
+      <c r="F1" t="s">
+        <v>26</v>
+      </c>
+      <c r="G1" t="s">
+        <v>27</v>
+      </c>
+      <c r="H1" t="s">
+        <v>34</v>
+      </c>
+      <c r="I1" t="s">
+        <v>35</v>
+      </c>
+      <c r="J1" t="s">
+        <v>23</v>
+      </c>
     </row>
     <row r="2" ht="14.25">
       <c r="A2" s="1">
-        <v>-0.44900000000000001</v>
+        <v>0.44900000000000001</v>
       </c>
       <c r="B2" s="1">
         <v>0.46600000000000003</v>
@@ -1845,61 +1893,253 @@
       <c r="D2" s="1">
         <v>0.27000000000000002</v>
       </c>
+      <c r="E2" s="6">
+        <f>0.5*($D$2)*B2*B2</f>
+        <v>0.029316060000000005</v>
+      </c>
+      <c r="F2" s="6">
+        <f>0.5*$C$2*A2*A2</f>
+        <v>0.027518536500000003</v>
+      </c>
+      <c r="G2" s="1">
+        <f>F2-E2</f>
+        <v>-0.001797523500000002</v>
+      </c>
+      <c r="H2" s="6">
+        <f>$D$2*B2</f>
+        <v>0.12582000000000002</v>
+      </c>
+      <c r="I2" s="6">
+        <f>$C$2*A2</f>
+        <v>0.12257700000000001</v>
+      </c>
+      <c r="J2" s="1">
+        <f>I2-H2</f>
+        <v>-0.0032430000000000098</v>
+      </c>
     </row>
     <row r="3" ht="14.25">
       <c r="A3" s="1">
-        <v>-0.63</v>
+        <v>0.63</v>
       </c>
       <c r="B3" s="1">
         <v>0.65800000000000003</v>
       </c>
+      <c r="E3" s="6">
+        <f>0.5*($D$2)*B3*B3</f>
+        <v>0.058450140000000005</v>
+      </c>
+      <c r="F3" s="6">
+        <f>0.5*$C$2*A3*A3</f>
+        <v>0.054176849999999999</v>
+      </c>
+      <c r="G3" s="1">
+        <f>F3-E3</f>
+        <v>-0.004273290000000006</v>
+      </c>
+      <c r="H3" s="6">
+        <f>$D$2*B3</f>
+        <v>0.17766000000000001</v>
+      </c>
+      <c r="I3" s="6">
+        <f>$C$2*A3</f>
+        <v>0.17199</v>
+      </c>
+      <c r="J3" s="1">
+        <f>I3-H3</f>
+        <v>-0.0056700000000000084</v>
+      </c>
     </row>
     <row r="4" ht="14.25">
       <c r="A4" s="1">
-        <v>-0.624</v>
+        <v>0.624</v>
       </c>
       <c r="B4" s="1">
         <v>0.64800000000000002</v>
       </c>
+      <c r="E4" s="6">
+        <f>0.5*($D$2)*B4*B4</f>
+        <v>0.056687040000000001</v>
+      </c>
+      <c r="F4" s="6">
+        <f>0.5*$C$2*A4*A4</f>
+        <v>0.053149823999999998</v>
+      </c>
+      <c r="G4" s="1">
+        <f>F4-E4</f>
+        <v>-0.0035372160000000027</v>
+      </c>
+      <c r="H4" s="6">
+        <f>$D$2*B4</f>
+        <v>0.17496</v>
+      </c>
+      <c r="I4" s="6">
+        <f>$C$2*A4</f>
+        <v>0.170352</v>
+      </c>
+      <c r="J4" s="1">
+        <f>I4-H4</f>
+        <v>-0.004608000000000001</v>
+      </c>
     </row>
     <row r="5" ht="14.25">
       <c r="A5" s="1">
-        <v>-0.56999999999999995</v>
+        <v>0.56999999999999995</v>
       </c>
       <c r="B5" s="1">
         <v>0.59399999999999997</v>
       </c>
+      <c r="E5" s="6">
+        <f>0.5*($D$2)*B5*B5</f>
+        <v>0.047632859999999999</v>
+      </c>
+      <c r="F5" s="6">
+        <f>0.5*$C$2*A5*A5</f>
+        <v>0.044348849999999995</v>
+      </c>
+      <c r="G5" s="1">
+        <f>F5-E5</f>
+        <v>-0.0032840100000000039</v>
+      </c>
+      <c r="H5" s="6">
+        <f>$D$2*B5</f>
+        <v>0.16037999999999999</v>
+      </c>
+      <c r="I5" s="6">
+        <f>$C$2*A5</f>
+        <v>0.15561</v>
+      </c>
+      <c r="J5" s="1">
+        <f>I5-H5</f>
+        <v>-0.0047699999999999965</v>
+      </c>
     </row>
     <row r="6" ht="14.25">
       <c r="A6" s="1">
-        <v>-0.58799999999999997</v>
+        <v>0.58799999999999997</v>
       </c>
       <c r="B6" s="1">
         <v>0.60899999999999999</v>
       </c>
+      <c r="E6" s="6">
+        <f>0.5*($D$2)*B6*B6</f>
+        <v>0.050068935000000002</v>
+      </c>
+      <c r="F6" s="6">
+        <f>0.5*$C$2*A6*A6</f>
+        <v>0.047194055999999998</v>
+      </c>
+      <c r="G6" s="1">
+        <f>F6-E6</f>
+        <v>-0.0028748790000000038</v>
+      </c>
+      <c r="H6" s="6">
+        <f>$D$2*B6</f>
+        <v>0.16443000000000002</v>
+      </c>
+      <c r="I6" s="6">
+        <f>$C$2*A6</f>
+        <v>0.160524</v>
+      </c>
+      <c r="J6" s="1">
+        <f>I6-H6</f>
+        <v>-0.0039060000000000206</v>
+      </c>
     </row>
     <row r="7" ht="14.25">
       <c r="A7" s="1">
-        <v>-0.80900000000000005</v>
+        <v>0.80900000000000005</v>
       </c>
       <c r="B7" s="1">
-        <v>0.88700000000000001</v>
+        <v>0.83699999999999997</v>
+      </c>
+      <c r="E7" s="6">
+        <f>0.5*($D$2)*B7*B7</f>
+        <v>0.094576814999999995</v>
+      </c>
+      <c r="F7" s="6">
+        <f>0.5*$C$2*A7*A7</f>
+        <v>0.089336656500000014</v>
+      </c>
+      <c r="G7" s="1">
+        <f>F7-E7</f>
+        <v>-0.0052401584999999806</v>
+      </c>
+      <c r="H7" s="6">
+        <f>$D$2*B7</f>
+        <v>0.22599</v>
+      </c>
+      <c r="I7" s="6">
+        <f>$C$2*A7</f>
+        <v>0.22085700000000003</v>
+      </c>
+      <c r="J7" s="1">
+        <f>I7-H7</f>
+        <v>-0.0051329999999999709</v>
       </c>
     </row>
     <row r="8" ht="14.25">
       <c r="A8" s="1">
-        <v>-0.86299999999999999</v>
+        <v>0.86299999999999999</v>
       </c>
       <c r="B8" s="1">
-        <v>0.96799999999999997</v>
+        <v>0.878</v>
+      </c>
+      <c r="E8" s="6">
+        <f>0.5*($D$2)*B8*B8</f>
+        <v>0.10406934000000001</v>
+      </c>
+      <c r="F8" s="6">
+        <f>0.5*$C$2*A8*A8</f>
+        <v>0.1016609685</v>
+      </c>
+      <c r="G8" s="1">
+        <f>F8-E8</f>
+        <v>-0.0024083715000000061</v>
+      </c>
+      <c r="H8" s="6">
+        <f>$D$2*B8</f>
+        <v>0.23706000000000002</v>
+      </c>
+      <c r="I8" s="6">
+        <f>$C$2*A8</f>
+        <v>0.235599</v>
+      </c>
+      <c r="J8" s="1">
+        <f>I8-H8</f>
+        <v>-0.0014610000000000178</v>
       </c>
     </row>
     <row r="9" ht="14.25">
       <c r="A9" s="1">
-        <v>-0.66300000000000003</v>
+        <v>0.66300000000000003</v>
       </c>
       <c r="B9" s="1">
         <v>0.69099999999999995</v>
+      </c>
+      <c r="E9" s="6">
+        <f>0.5*($D$2)*B9*B9</f>
+        <v>0.064459934999999996</v>
+      </c>
+      <c r="F9" s="6">
+        <f>0.5*$C$2*A9*A9</f>
+        <v>0.060001168500000007</v>
+      </c>
+      <c r="G9" s="1">
+        <f>F9-E9</f>
+        <v>-0.0044587664999999888</v>
+      </c>
+      <c r="H9" s="6">
+        <f>$D$2*B9</f>
+        <v>0.18656999999999999</v>
+      </c>
+      <c r="I9" s="6">
+        <f>$C$2*A9</f>
+        <v>0.18099900000000002</v>
+      </c>
+      <c r="J9" s="1">
+        <f>I9-H9</f>
+        <v>-0.0055709999999999649</v>
       </c>
     </row>
     <row r="10" ht="14.25">
@@ -1926,24 +2166,52 @@
   <sheetData>
     <row r="1">
       <c r="A1" t="s">
+        <v>36</v>
+      </c>
+      <c r="B1" t="s">
+        <v>37</v>
+      </c>
+      <c r="C1" t="s">
+        <v>38</v>
+      </c>
+      <c r="D1" t="s">
+        <v>39</v>
+      </c>
+      <c r="E1" t="s">
+        <v>40</v>
+      </c>
+      <c r="F1" t="s">
+        <v>25</v>
+      </c>
+      <c r="G1" t="s">
+        <v>26</v>
+      </c>
+      <c r="H1" t="s">
+        <v>27</v>
+      </c>
+      <c r="I1" t="s">
+        <v>41</v>
+      </c>
+      <c r="J1" t="s">
+        <v>42</v>
+      </c>
+      <c r="K1" t="s">
         <v>34</v>
       </c>
-      <c r="B1" t="s">
+      <c r="L1" t="s">
         <v>35</v>
       </c>
-      <c r="C1" t="s">
-        <v>36</v>
-      </c>
-      <c r="D1" t="s">
-        <v>37</v>
-      </c>
-      <c r="E1" t="s">
-        <v>38</v>
+      <c r="M1" t="s">
+        <v>23</v>
       </c>
     </row>
     <row r="2">
-      <c r="A2" s="1"/>
-      <c r="B2" s="1"/>
+      <c r="A2" s="1">
+        <v>-0.37</v>
+      </c>
+      <c r="B2" s="1">
+        <v>-0.17799999999999999</v>
+      </c>
       <c r="C2" s="1">
         <v>0.25</v>
       </c>
@@ -1953,38 +2221,506 @@
       <c r="E2">
         <v>0</v>
       </c>
+      <c r="F2" s="6">
+        <f>0.5*$D$2*A2*A2</f>
+        <v>0.016907149999999999</v>
+      </c>
+      <c r="G2" s="6">
+        <f>0.5*($C$2+$D$2)*B2*B2</f>
+        <v>0.0078734739999999984</v>
+      </c>
+      <c r="H2" s="1">
+        <f>G2-F2</f>
+        <v>-0.0090336760000000009</v>
+      </c>
+      <c r="I2" s="1">
+        <f>B2-A2</f>
+        <v>0.192</v>
+      </c>
+      <c r="J2" s="8">
+        <f>I2/A2</f>
+        <v>-0.51891891891891895</v>
+      </c>
+      <c r="K2" s="1">
+        <f>$D$2*A2</f>
+        <v>-0.091389999999999999</v>
+      </c>
+      <c r="L2" s="1">
+        <f>($C$2+$D$2)*B2</f>
+        <v>-0.088465999999999989</v>
+      </c>
+      <c r="M2" s="1">
+        <f>L2-K2</f>
+        <v>0.0029240000000000099</v>
+      </c>
     </row>
     <row r="3">
-      <c r="A3" s="1"/>
-      <c r="B3" s="1"/>
+      <c r="A3" s="1">
+        <v>-0.502</v>
+      </c>
+      <c r="B3" s="1">
+        <v>-0.24299999999999999</v>
+      </c>
+      <c r="F3" s="6">
+        <f>0.5*$D$2*A3*A3</f>
+        <v>0.031122493999999997</v>
+      </c>
+      <c r="G3" s="6">
+        <f>0.5*($C$2+$D$2)*B3*B3</f>
+        <v>0.014673676499999998</v>
+      </c>
+      <c r="H3" s="1">
+        <f>G3-F3</f>
+        <v>-0.016448817499999997</v>
+      </c>
+      <c r="I3" s="1">
+        <f>B3-A3</f>
+        <v>0.25900000000000001</v>
+      </c>
+      <c r="J3" s="8">
+        <f>I3/A3</f>
+        <v>-0.51593625498007967</v>
+      </c>
+      <c r="K3" s="1">
+        <f>$D$2*A3</f>
+        <v>-0.12399399999999999</v>
+      </c>
+      <c r="L3" s="1">
+        <f>($C$2+$D$2)*B3</f>
+        <v>-0.12077099999999999</v>
+      </c>
+      <c r="M3" s="1">
+        <f>L3-K3</f>
+        <v>0.0032230000000000036</v>
+      </c>
     </row>
     <row r="4">
-      <c r="A4" s="1"/>
-      <c r="B4" s="1"/>
+      <c r="A4" s="1">
+        <v>-0.61499999999999999</v>
+      </c>
+      <c r="B4" s="1">
+        <v>-0.30199999999999999</v>
+      </c>
+      <c r="F4" s="6">
+        <f>0.5*$D$2*A4*A4</f>
+        <v>0.046710787499999996</v>
+      </c>
+      <c r="G4" s="6">
+        <f>0.5*($C$2+$D$2)*B4*B4</f>
+        <v>0.022664193999999999</v>
+      </c>
+      <c r="H4" s="1">
+        <f>G4-F4</f>
+        <v>-0.024046593499999998</v>
+      </c>
+      <c r="I4" s="1">
+        <f>B4-A4</f>
+        <v>0.313</v>
+      </c>
+      <c r="J4" s="8">
+        <f>I4/A4</f>
+        <v>-0.50894308943089428</v>
+      </c>
+      <c r="K4" s="1">
+        <f>$D$2*A4</f>
+        <v>-0.15190499999999998</v>
+      </c>
+      <c r="L4" s="1">
+        <f>($C$2+$D$2)*B4</f>
+        <v>-0.15009400000000001</v>
+      </c>
+      <c r="M4" s="1">
+        <f>L4-K4</f>
+        <v>0.0018109999999999793</v>
+      </c>
     </row>
     <row r="5">
-      <c r="A5" s="1"/>
-      <c r="B5" s="1"/>
+      <c r="A5" s="1">
+        <v>-0.65600000000000003</v>
+      </c>
+      <c r="B5" s="1">
+        <v>-0.32000000000000001</v>
+      </c>
+      <c r="F5" s="6">
+        <f>0.5*$D$2*A5*A5</f>
+        <v>0.053146496000000008</v>
+      </c>
+      <c r="G5" s="6">
+        <f>0.5*($C$2+$D$2)*B5*B5</f>
+        <v>0.025446400000000004</v>
+      </c>
+      <c r="H5" s="1">
+        <f>G5-F5</f>
+        <v>-0.027700096000000004</v>
+      </c>
+      <c r="I5" s="1">
+        <f>B5-A5</f>
+        <v>0.33600000000000002</v>
+      </c>
+      <c r="J5" s="8">
+        <f>I5/A5</f>
+        <v>-0.51219512195121952</v>
+      </c>
+      <c r="K5" s="1">
+        <f>$D$2*A5</f>
+        <v>-0.16203200000000001</v>
+      </c>
+      <c r="L5" s="1">
+        <f>($C$2+$D$2)*B5</f>
+        <v>-0.15904000000000001</v>
+      </c>
+      <c r="M5" s="1">
+        <f>L5-K5</f>
+        <v>0.0029919999999999947</v>
+      </c>
     </row>
     <row r="6">
-      <c r="A6" s="1"/>
-      <c r="B6" s="1"/>
+      <c r="A6" s="1">
+        <v>-0.54700000000000004</v>
+      </c>
+      <c r="B6" s="1">
+        <v>-0.26400000000000001</v>
+      </c>
+      <c r="F6" s="6">
+        <f>0.5*$D$2*A6*A6</f>
+        <v>0.036952311500000001</v>
+      </c>
+      <c r="G6" s="6">
+        <f>0.5*($C$2+$D$2)*B6*B6</f>
+        <v>0.017319456000000004</v>
+      </c>
+      <c r="H6" s="1">
+        <f>G6-F6</f>
+        <v>-0.019632855499999997</v>
+      </c>
+      <c r="I6" s="1">
+        <f>B6-A6</f>
+        <v>0.28300000000000003</v>
+      </c>
+      <c r="J6" s="8">
+        <f>I6/A6</f>
+        <v>-0.51736745886654478</v>
+      </c>
+      <c r="K6" s="1">
+        <f>$D$2*A6</f>
+        <v>-0.13510900000000001</v>
+      </c>
+      <c r="L6" s="1">
+        <f>($C$2+$D$2)*B6</f>
+        <v>-0.13120800000000002</v>
+      </c>
+      <c r="M6" s="1">
+        <f>L6-K6</f>
+        <v>0.0039009999999999878</v>
+      </c>
     </row>
     <row r="7">
-      <c r="A7" s="1"/>
-      <c r="B7" s="1"/>
+      <c r="A7" s="1">
+        <v>-0.67900000000000005</v>
+      </c>
+      <c r="B7" s="1">
+        <v>-0.33000000000000002</v>
+      </c>
+      <c r="F7" s="6">
+        <f>0.5*$D$2*A7*A7</f>
+        <v>0.056938563500000004</v>
+      </c>
+      <c r="G7" s="6">
+        <f>0.5*($C$2+$D$2)*B7*B7</f>
+        <v>0.027061650000000003</v>
+      </c>
+      <c r="H7" s="1">
+        <f>G7-F7</f>
+        <v>-0.029876913500000001</v>
+      </c>
+      <c r="I7" s="1">
+        <f>B7-A7</f>
+        <v>0.34900000000000003</v>
+      </c>
+      <c r="J7" s="8">
+        <f>I7/A7</f>
+        <v>-0.51399116347569962</v>
+      </c>
+      <c r="K7" s="1">
+        <f>$D$2*A7</f>
+        <v>-0.167713</v>
+      </c>
+      <c r="L7" s="1">
+        <f>($C$2+$D$2)*B7</f>
+        <v>-0.16401000000000002</v>
+      </c>
+      <c r="M7" s="1">
+        <f>L7-K7</f>
+        <v>0.0037029999999999841</v>
+      </c>
     </row>
     <row r="8">
-      <c r="A8" s="1"/>
-      <c r="B8" s="1"/>
+      <c r="A8" s="1">
+        <v>-0.55600000000000005</v>
+      </c>
+      <c r="B8" s="1">
+        <v>-0.26900000000000002</v>
+      </c>
+      <c r="F8" s="6">
+        <f>0.5*$D$2*A8*A8</f>
+        <v>0.038178296000000007</v>
+      </c>
+      <c r="G8" s="6">
+        <f>0.5*($C$2+$D$2)*B8*B8</f>
+        <v>0.017981708500000002</v>
+      </c>
+      <c r="H8" s="1">
+        <f>G8-F8</f>
+        <v>-0.020196587500000005</v>
+      </c>
+      <c r="I8" s="1">
+        <f>B8-A8</f>
+        <v>0.28700000000000003</v>
+      </c>
+      <c r="J8" s="8">
+        <f>I8/A8</f>
+        <v>-0.51618705035971224</v>
+      </c>
+      <c r="K8" s="1">
+        <f>$D$2*A8</f>
+        <v>-0.13733200000000001</v>
+      </c>
+      <c r="L8" s="1">
+        <f>($C$2+$D$2)*B8</f>
+        <v>-0.13369300000000001</v>
+      </c>
+      <c r="M8" s="1">
+        <f>L8-K8</f>
+        <v>0.0036390000000000033</v>
+      </c>
     </row>
     <row r="9">
-      <c r="A9" s="1"/>
-      <c r="B9" s="1"/>
+      <c r="A9" s="1">
+        <v>-0.53500000000000003</v>
+      </c>
+      <c r="B9" s="1">
+        <v>-0.26000000000000001</v>
+      </c>
+      <c r="F9" s="6">
+        <f>0.5*$D$2*A9*A9</f>
+        <v>0.035348787500000006</v>
+      </c>
+      <c r="G9" s="6">
+        <f>0.5*($C$2+$D$2)*B9*B9</f>
+        <v>0.0167986</v>
+      </c>
+      <c r="H9" s="1">
+        <f>G9-F9</f>
+        <v>-0.018550187500000006</v>
+      </c>
+      <c r="I9" s="1">
+        <f>B9-A9</f>
+        <v>0.27500000000000002</v>
+      </c>
+      <c r="J9" s="8">
+        <f>I9/A9</f>
+        <v>-0.5140186915887851</v>
+      </c>
+      <c r="K9" s="1">
+        <f>$D$2*A9</f>
+        <v>-0.13214500000000001</v>
+      </c>
+      <c r="L9" s="1">
+        <f>($C$2+$D$2)*B9</f>
+        <v>-0.12922</v>
+      </c>
+      <c r="M9" s="1">
+        <f>L9-K9</f>
+        <v>0.0029250000000000109</v>
+      </c>
     </row>
     <row r="10">
-      <c r="A10" s="1"/>
-      <c r="B10" s="1"/>
+      <c r="A10" s="1">
+        <v>-0.55600000000000005</v>
+      </c>
+      <c r="B10" s="1">
+        <v>-0.27000000000000002</v>
+      </c>
+      <c r="F10" s="6">
+        <f>0.5*$D$2*A10*A10</f>
+        <v>0.038178296000000007</v>
+      </c>
+      <c r="G10" s="6">
+        <f>0.5*($C$2+$D$2)*B10*B10</f>
+        <v>0.018115650000000001</v>
+      </c>
+      <c r="H10" s="1">
+        <f>G10-F10</f>
+        <v>-0.020062646000000007</v>
+      </c>
+      <c r="I10" s="1">
+        <f>B10-A10</f>
+        <v>0.28600000000000003</v>
+      </c>
+      <c r="J10" s="8">
+        <f>I10/A10</f>
+        <v>-0.51438848920863312</v>
+      </c>
+      <c r="K10" s="1">
+        <f>$D$2*A10</f>
+        <v>-0.13733200000000001</v>
+      </c>
+      <c r="L10" s="1">
+        <f>($C$2+$D$2)*B10</f>
+        <v>-0.13419</v>
+      </c>
+      <c r="M10" s="1">
+        <f>L10-K10</f>
+        <v>0.0031420000000000059</v>
+      </c>
+    </row>
+  </sheetData>
+  <printOptions headings="0" gridLines="0"/>
+  <pageMargins left="0.70078740157480324" right="0.70078740157480324" top="0.75196850393700787" bottom="0.75196850393700787" header="0.29999999999999999" footer="0.29999999999999999"/>
+  <pageSetup paperSize="9" scale="100" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" usePrinterDefaults="1" blackAndWhite="0" draft="0" cellComments="none" useFirstPageNumber="0" errors="displayed" horizontalDpi="600" verticalDpi="600" copies="1"/>
+  <headerFooter/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac">
+  <sheetViews>
+    <sheetView zoomScale="100" workbookViewId="0">
+      <selection activeCell="A1" activeCellId="0" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetData>
+    <row r="1">
+      <c r="A1" t="s">
+        <v>31</v>
+      </c>
+      <c r="B1" t="s">
+        <v>22</v>
+      </c>
+      <c r="I1" t="s">
+        <v>38</v>
+      </c>
+      <c r="J1" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="2">
+      <c r="A2" s="1">
+        <v>0.66000000000000003</v>
+      </c>
+      <c r="B2" s="1">
+        <v>0.21199999999999999</v>
+      </c>
+      <c r="I2" s="1">
+        <v>0.503</v>
+      </c>
+      <c r="J2" s="1">
+        <v>0.247</v>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" s="1">
+        <v>0.61799999999999999</v>
+      </c>
+      <c r="B3" s="1">
+        <v>0.19900000000000001</v>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" s="1">
+        <v>0.71499999999999997</v>
+      </c>
+      <c r="B4" s="1">
+        <v>0.23100000000000001</v>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" s="1">
+        <v>0.63600000000000001</v>
+      </c>
+      <c r="B5" s="1">
+        <v>0.20499999999999999</v>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" s="1">
+        <v>0.39800000000000002</v>
+      </c>
+      <c r="B6" s="1">
+        <v>0.125</v>
+      </c>
+    </row>
+    <row r="7">
+      <c r="A7" s="1">
+        <v>0.40400000000000003</v>
+      </c>
+      <c r="B7" s="1">
+        <v>0.128</v>
+      </c>
+    </row>
+    <row r="8">
+      <c r="A8" s="1">
+        <v>0.36599999999999999</v>
+      </c>
+      <c r="B8" s="1">
+        <v>0.11600000000000001</v>
+      </c>
+    </row>
+    <row r="9">
+      <c r="A9" s="1">
+        <v>0.309</v>
+      </c>
+      <c r="B9" s="1">
+        <v>0.097000000000000003</v>
+      </c>
+    </row>
+    <row r="10">
+      <c r="A10" s="1">
+        <v>0.28699999999999998</v>
+      </c>
+      <c r="B10" s="1">
+        <v>0.089999999999999997</v>
+      </c>
+    </row>
+    <row r="11">
+      <c r="A11">
+        <v>0.35199999999999998</v>
+      </c>
+      <c r="B11">
+        <v>0.112</v>
+      </c>
+    </row>
+  </sheetData>
+  <printOptions headings="0" gridLines="0"/>
+  <pageMargins left="0.70078740157480324" right="0.70078740157480324" top="0.75196850393700787" bottom="0.75196850393700787" header="0.29999999999999999" footer="0.29999999999999999"/>
+  <pageSetup paperSize="9" scale="100" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" usePrinterDefaults="1" blackAndWhite="0" draft="0" cellComments="none" useFirstPageNumber="0" errors="displayed" horizontalDpi="600" verticalDpi="600" copies="1"/>
+  <headerFooter/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac">
+  <sheetViews>
+    <sheetView zoomScale="100" workbookViewId="0">
+      <selection activeCell="A1" activeCellId="0" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetData>
+    <row r="1">
+      <c r="A1" t="s">
+        <v>31</v>
+      </c>
+      <c r="B1" t="s">
+        <v>30</v>
+      </c>
+      <c r="I1" t="s">
+        <v>38</v>
+      </c>
+      <c r="J1" t="s">
+        <v>39</v>
+      </c>
     </row>
   </sheetData>
   <printOptions headings="0" gridLines="0"/>

</xml_diff>

<commit_message>
rivedere con la Marta il piano inclinato
</commit_message>
<xml_diff>
--- a/URTI/urti_dati.xlsx
+++ b/URTI/urti_dati.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <workbookPr/>
   <bookViews>
-    <workbookView xWindow="360" yWindow="15" windowWidth="20955" windowHeight="9720" activeTab="2"/>
+    <workbookView xWindow="360" yWindow="15" windowWidth="20955" windowHeight="9720" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" state="visible" r:id="rId1"/>
@@ -204,7 +204,6 @@
     </font>
     <font>
       <sz val="11.000000"/>
-      <color indexed="64"/>
       <name val="Calibri"/>
     </font>
   </fonts>
@@ -226,16 +225,16 @@
     </border>
     <border>
       <left style="thin">
-        <color indexed="64"/>
+        <color auto="1"/>
       </left>
       <right style="thin">
-        <color indexed="64"/>
+        <color auto="1"/>
       </right>
       <top style="thin">
-        <color indexed="64"/>
+        <color auto="1"/>
       </top>
       <bottom style="thin">
-        <color indexed="64"/>
+        <color auto="1"/>
       </bottom>
       <diagonal/>
     </border>
@@ -243,7 +242,7 @@
   <cellStyleXfs count="1">
     <xf fontId="0" fillId="0" borderId="0" numFmtId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
   </cellStyleXfs>
-  <cellXfs count="34">
+  <cellXfs count="36">
     <xf fontId="0" fillId="0" borderId="0" numFmtId="0" xfId="0"/>
     <xf fontId="0" fillId="0" borderId="0" numFmtId="0" xfId="0"/>
     <xf fontId="0" fillId="0" borderId="0" numFmtId="160" xfId="0" applyNumberFormat="1" applyAlignment="1">
@@ -270,14 +269,17 @@
     <xf fontId="2" fillId="0" borderId="0" numFmtId="161" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf fontId="2" fillId="0" borderId="0" numFmtId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
     <xf fontId="0" fillId="0" borderId="0" numFmtId="4" xfId="0" applyNumberFormat="1"/>
     <xf fontId="0" fillId="0" borderId="0" numFmtId="160" xfId="0" applyNumberFormat="1"/>
     <xf fontId="0" fillId="0" borderId="0" numFmtId="161" xfId="0" applyNumberFormat="1"/>
     <xf fontId="0" fillId="0" borderId="0" numFmtId="3" xfId="0" applyNumberFormat="1"/>
     <xf fontId="0" fillId="0" borderId="0" numFmtId="0" xfId="0">
+      <protection hidden="0" locked="1"/>
+    </xf>
+    <xf fontId="0" fillId="0" borderId="0" numFmtId="162" xfId="0" applyNumberFormat="1">
+      <protection hidden="0" locked="1"/>
+    </xf>
+    <xf fontId="0" fillId="0" borderId="0" numFmtId="163" xfId="0" applyNumberFormat="1">
       <protection hidden="0" locked="1"/>
     </xf>
     <xf fontId="0" fillId="0" borderId="0" numFmtId="162" xfId="0" applyNumberFormat="1"/>
@@ -288,6 +290,9 @@
     </xf>
     <xf fontId="1" fillId="0" borderId="0" numFmtId="164" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="left"/>
+    </xf>
+    <xf fontId="2" fillId="0" borderId="0" numFmtId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="right"/>
     </xf>
     <xf fontId="2" fillId="0" borderId="0" numFmtId="164" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="right"/>
@@ -892,24 +897,24 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25"/>
   <cols>
-    <col bestFit="1" customWidth="1" min="1" max="1" style="31" width="12.43357142857143"/>
-    <col bestFit="1" customWidth="1" min="2" max="2" style="25" width="12.43357142857143"/>
-    <col bestFit="1" customWidth="1" min="3" max="3" style="31" width="12.43357142857143"/>
-    <col bestFit="1" customWidth="1" min="4" max="4" style="25" width="12.43357142857143"/>
-    <col bestFit="1" customWidth="1" min="5" max="6" style="12" width="12.43357142857143"/>
+    <col bestFit="1" customWidth="1" min="1" max="1" style="33" width="12.43357142857143"/>
+    <col bestFit="1" customWidth="1" min="2" max="2" style="27" width="12.43357142857143"/>
+    <col bestFit="1" customWidth="1" min="3" max="3" style="33" width="12.43357142857143"/>
+    <col bestFit="1" customWidth="1" min="4" max="4" style="27" width="12.43357142857143"/>
+    <col bestFit="1" customWidth="1" min="5" max="6" style="11" width="12.43357142857143"/>
   </cols>
   <sheetData>
     <row r="1" ht="17.25" customHeight="1">
-      <c r="A1" s="32" t="s">
+      <c r="A1" s="34" t="s">
         <v>44</v>
       </c>
-      <c r="B1" s="19" t="s">
+      <c r="B1" s="20" t="s">
         <v>45</v>
       </c>
-      <c r="C1" s="32" t="s">
+      <c r="C1" s="34" t="s">
         <v>46</v>
       </c>
-      <c r="D1" s="19" t="s">
+      <c r="D1" s="20" t="s">
         <v>47</v>
       </c>
       <c r="E1" s="5" t="s">
@@ -920,17 +925,17 @@
       </c>
     </row>
     <row r="2" ht="17.25" customHeight="1">
-      <c r="A2" s="33">
+      <c r="A2" s="35">
         <v>1.1000000000000001</v>
       </c>
-      <c r="B2" s="10">
+      <c r="B2" s="22">
         <f t="shared" ref="B2:B7" si="26">A2/($E$2*9.81)</f>
         <v>0.22426095820591235</v>
       </c>
-      <c r="C2" s="33">
+      <c r="C2" s="35">
         <v>1.3</v>
       </c>
-      <c r="D2" s="10">
+      <c r="D2" s="22">
         <f t="shared" ref="D2:D7" si="27">C2/($F$2*9.81)</f>
         <v>0.20231731135856074</v>
       </c>
@@ -942,110 +947,110 @@
       </c>
     </row>
     <row r="3" ht="17.25" customHeight="1">
-      <c r="A3" s="33">
+      <c r="A3" s="35">
         <v>1.1000000000000001</v>
       </c>
-      <c r="B3" s="10">
+      <c r="B3" s="22">
         <f t="shared" si="26"/>
         <v>0.22426095820591235</v>
       </c>
-      <c r="C3" s="33">
+      <c r="C3" s="35">
         <v>1.3999999999999999</v>
       </c>
-      <c r="D3" s="10">
+      <c r="D3" s="22">
         <f t="shared" si="27"/>
         <v>0.2178801814630654</v>
       </c>
-      <c r="E3" s="23"/>
-      <c r="F3" s="23"/>
+      <c r="E3" s="25"/>
+      <c r="F3" s="25"/>
     </row>
     <row r="4" ht="17.25" customHeight="1">
-      <c r="A4" s="33">
+      <c r="A4" s="35">
         <v>0.90000000000000002</v>
       </c>
-      <c r="B4" s="10">
+      <c r="B4" s="22">
         <f t="shared" si="26"/>
         <v>0.18348623853211007</v>
       </c>
-      <c r="C4" s="33">
+      <c r="C4" s="35">
         <v>1.3999999999999999</v>
       </c>
-      <c r="D4" s="10">
+      <c r="D4" s="22">
         <f t="shared" si="27"/>
         <v>0.2178801814630654</v>
       </c>
-      <c r="E4" s="23"/>
-      <c r="F4" s="23"/>
+      <c r="E4" s="25"/>
+      <c r="F4" s="25"/>
     </row>
     <row r="5" ht="17.25" customHeight="1">
-      <c r="A5" s="33">
+      <c r="A5" s="35">
         <v>1.2</v>
       </c>
-      <c r="B5" s="10">
+      <c r="B5" s="22">
         <f t="shared" si="26"/>
         <v>0.24464831804281342</v>
       </c>
-      <c r="C5" s="33">
+      <c r="C5" s="35">
         <v>1.5</v>
       </c>
-      <c r="D5" s="10">
+      <c r="D5" s="22">
         <f t="shared" si="27"/>
         <v>0.23344305156757009</v>
       </c>
-      <c r="E5" s="23"/>
-      <c r="F5" s="23"/>
+      <c r="E5" s="25"/>
+      <c r="F5" s="25"/>
     </row>
     <row r="6" ht="17.25" customHeight="1">
-      <c r="A6" s="33">
+      <c r="A6" s="35">
         <v>1.2</v>
       </c>
-      <c r="B6" s="10">
+      <c r="B6" s="22">
         <f t="shared" si="26"/>
         <v>0.24464831804281342</v>
       </c>
-      <c r="C6" s="33">
+      <c r="C6" s="35">
         <v>1.3</v>
       </c>
-      <c r="D6" s="10">
+      <c r="D6" s="22">
         <f t="shared" si="27"/>
         <v>0.20231731135856074</v>
       </c>
-      <c r="E6" s="23"/>
-      <c r="F6" s="23"/>
+      <c r="E6" s="25"/>
+      <c r="F6" s="25"/>
     </row>
     <row r="7" ht="17.25" customHeight="1">
-      <c r="A7" s="33">
+      <c r="A7" s="35">
         <v>1</v>
       </c>
-      <c r="B7" s="10">
+      <c r="B7" s="22">
         <f t="shared" si="26"/>
         <v>0.2038735983690112</v>
       </c>
-      <c r="C7" s="33">
+      <c r="C7" s="35">
         <v>1.3</v>
       </c>
-      <c r="D7" s="10">
+      <c r="D7" s="22">
         <f t="shared" si="27"/>
         <v>0.20231731135856074</v>
       </c>
-      <c r="E7" s="23"/>
-      <c r="F7" s="23"/>
+      <c r="E7" s="25"/>
+      <c r="F7" s="25"/>
     </row>
     <row r="8" ht="17.25" customHeight="1">
-      <c r="A8" s="33"/>
-      <c r="B8" s="10"/>
-      <c r="C8" s="10"/>
-      <c r="D8" s="10"/>
-      <c r="E8" s="23"/>
-      <c r="F8" s="23"/>
+      <c r="A8" s="35"/>
+      <c r="B8" s="22"/>
+      <c r="C8" s="22"/>
+      <c r="D8" s="22"/>
+      <c r="E8" s="25"/>
+      <c r="F8" s="25"/>
     </row>
     <row r="9" ht="17.25" customHeight="1">
-      <c r="A9" s="33"/>
-      <c r="B9" s="10"/>
-      <c r="C9" s="10"/>
-      <c r="D9" s="10"/>
-      <c r="E9" s="23"/>
-      <c r="F9" s="23"/>
+      <c r="A9" s="35"/>
+      <c r="B9" s="22"/>
+      <c r="C9" s="22"/>
+      <c r="D9" s="22"/>
+      <c r="E9" s="25"/>
+      <c r="F9" s="25"/>
     </row>
   </sheetData>
   <printOptions headings="0" gridLines="0"/>
@@ -1069,94 +1074,94 @@
   <sheetFormatPr defaultRowHeight="14.25"/>
   <cols>
     <col bestFit="1" customWidth="1" min="1" max="1" style="4" width="12.43357142857143"/>
-    <col bestFit="1" customWidth="1" min="2" max="2" style="11" width="12.43357142857143"/>
-    <col bestFit="1" customWidth="1" min="3" max="3" style="14" width="12.43357142857143"/>
+    <col bestFit="1" customWidth="1" min="2" max="2" style="10" width="12.43357142857143"/>
+    <col bestFit="1" customWidth="1" min="3" max="3" style="13" width="12.43357142857143"/>
   </cols>
   <sheetData>
     <row r="1" ht="17.25" customHeight="1">
-      <c r="A1" s="22" t="s">
+      <c r="A1" s="24" t="s">
         <v>50</v>
       </c>
       <c r="B1" s="7" t="s">
         <v>28</v>
       </c>
-      <c r="C1" s="27" t="s">
+      <c r="C1" s="29" t="s">
         <v>18</v>
       </c>
     </row>
     <row r="2" ht="17.25" customHeight="1">
-      <c r="A2" s="10">
+      <c r="A2" s="22">
         <v>1.72</v>
       </c>
-      <c r="B2" s="10">
+      <c r="B2" s="22">
         <v>0.254</v>
       </c>
-      <c r="C2" s="28">
+      <c r="C2" s="30">
         <v>10</v>
       </c>
     </row>
     <row r="3" ht="17.25" customHeight="1">
-      <c r="A3" s="10">
+      <c r="A3" s="22">
         <v>1.73</v>
       </c>
-      <c r="B3" s="22"/>
-      <c r="C3" s="30"/>
+      <c r="B3" s="24"/>
+      <c r="C3" s="32"/>
     </row>
     <row r="4" ht="17.25" customHeight="1">
-      <c r="A4" s="10">
+      <c r="A4" s="22">
         <v>1.7</v>
       </c>
-      <c r="B4" s="22"/>
-      <c r="C4" s="30"/>
+      <c r="B4" s="24"/>
+      <c r="C4" s="32"/>
     </row>
     <row r="5" ht="17.25" customHeight="1">
-      <c r="A5" s="10">
+      <c r="A5" s="22">
         <v>1.71</v>
       </c>
-      <c r="B5" s="22"/>
-      <c r="C5" s="30"/>
+      <c r="B5" s="24"/>
+      <c r="C5" s="32"/>
     </row>
     <row r="6" ht="17.25" customHeight="1">
-      <c r="A6" s="10">
+      <c r="A6" s="22">
         <v>1.7</v>
       </c>
-      <c r="B6" s="22"/>
-      <c r="C6" s="30"/>
+      <c r="B6" s="24"/>
+      <c r="C6" s="32"/>
     </row>
     <row r="7" ht="17.25" customHeight="1">
-      <c r="A7" s="10">
+      <c r="A7" s="22">
         <v>1.73</v>
       </c>
-      <c r="B7" s="22"/>
-      <c r="C7" s="30"/>
+      <c r="B7" s="24"/>
+      <c r="C7" s="32"/>
     </row>
     <row r="8" ht="17.25" customHeight="1">
-      <c r="A8" s="10">
+      <c r="A8" s="22">
         <v>1.73</v>
       </c>
-      <c r="B8" s="22"/>
-      <c r="C8" s="30"/>
+      <c r="B8" s="24"/>
+      <c r="C8" s="32"/>
     </row>
     <row r="9" ht="17.25" customHeight="1">
-      <c r="A9" s="10">
+      <c r="A9" s="22">
         <v>1.72</v>
       </c>
-      <c r="B9" s="22"/>
-      <c r="C9" s="30"/>
+      <c r="B9" s="24"/>
+      <c r="C9" s="32"/>
     </row>
     <row r="10" ht="17.25" customHeight="1">
-      <c r="A10" s="10">
+      <c r="A10" s="22">
         <v>1.73</v>
       </c>
-      <c r="B10" s="22"/>
-      <c r="C10" s="30"/>
+      <c r="B10" s="24"/>
+      <c r="C10" s="32"/>
     </row>
     <row r="11" ht="17.25" customHeight="1">
-      <c r="A11" s="10">
+      <c r="A11" s="22">
         <v>1.73</v>
       </c>
-      <c r="B11" s="22"/>
-      <c r="C11" s="30"/>
+      <c r="B11" s="24"/>
+      <c r="C11" s="32"/>
     </row>
   </sheetData>
   <printOptions headings="0" gridLines="0"/>
@@ -1231,7 +1236,7 @@
       <c r="E2" s="8">
         <v>0.39400000000000002</v>
       </c>
-      <c r="F2" s="10">
+      <c r="F2" s="9">
         <v>0.0014</v>
       </c>
       <c r="G2" s="8">
@@ -1257,7 +1262,7 @@
       <c r="E3" s="8">
         <v>0.39200000000000002</v>
       </c>
-      <c r="F3" s="10">
+      <c r="F3" s="9">
         <v>0.0016000000000000001</v>
       </c>
       <c r="G3" s="8">
@@ -1283,7 +1288,7 @@
       <c r="E4" s="8">
         <v>0.38900000000000001</v>
       </c>
-      <c r="F4" s="10">
+      <c r="F4" s="9">
         <v>0.0014</v>
       </c>
       <c r="G4" s="8">
@@ -1295,7 +1300,7 @@
     </row>
     <row r="5" ht="18.75" customHeight="1">
       <c r="A5" s="8">
-        <v>0.26600000000000001</v>
+        <v>0.25600000000000001</v>
       </c>
       <c r="B5" s="9">
         <v>0.0019</v>
@@ -1309,7 +1314,7 @@
       <c r="E5" s="8">
         <v>0.39100000000000001</v>
       </c>
-      <c r="F5" s="10">
+      <c r="F5" s="9">
         <v>0.0016000000000000001</v>
       </c>
       <c r="G5" s="8">
@@ -1335,7 +1340,7 @@
       <c r="E6" s="8">
         <v>0.39000000000000001</v>
       </c>
-      <c r="F6" s="10">
+      <c r="F6" s="9">
         <v>0.0011999999999999999</v>
       </c>
       <c r="G6" s="8">
@@ -1361,7 +1366,7 @@
       <c r="E7" s="8">
         <v>0.39600000000000002</v>
       </c>
-      <c r="F7" s="10">
+      <c r="F7" s="9">
         <v>0.0015</v>
       </c>
       <c r="G7" s="8">
@@ -1387,7 +1392,7 @@
       <c r="E8" s="8">
         <v>0.39400000000000002</v>
       </c>
-      <c r="F8" s="10">
+      <c r="F8" s="9">
         <v>0.0012999999999999999</v>
       </c>
       <c r="G8" s="8">
@@ -1413,7 +1418,7 @@
       <c r="E9" s="8">
         <v>0.39100000000000001</v>
       </c>
-      <c r="F9" s="10">
+      <c r="F9" s="9">
         <v>0.0016000000000000001</v>
       </c>
       <c r="G9" s="8">
@@ -1439,7 +1444,7 @@
       <c r="E10" s="8">
         <v>0.39000000000000001</v>
       </c>
-      <c r="F10" s="10">
+      <c r="F10" s="9">
         <v>0.0014</v>
       </c>
       <c r="G10" s="8">
@@ -1465,7 +1470,7 @@
       <c r="E11" s="8">
         <v>0.39200000000000002</v>
       </c>
-      <c r="F11" s="10">
+      <c r="F11" s="9">
         <v>0.0012999999999999999</v>
       </c>
       <c r="G11" s="8">
@@ -1491,7 +1496,7 @@
       <c r="E12" s="8">
         <v>0.39400000000000002</v>
       </c>
-      <c r="F12" s="10">
+      <c r="F12" s="9">
         <v>0.0014</v>
       </c>
       <c r="G12" s="8">
@@ -1522,33 +1527,33 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25"/>
   <cols>
-    <col customWidth="1" min="1" max="1" style="11" width="10.00390625"/>
-    <col bestFit="1" customWidth="1" min="2" max="2" style="11" width="10.005000000000001"/>
-    <col bestFit="1" customWidth="1" min="3" max="3" style="12" width="12.43357142857143"/>
-    <col bestFit="1" customWidth="1" min="4" max="4" style="13" width="10.005000000000001"/>
-    <col bestFit="1" customWidth="1" min="5" max="7" style="14" width="12.43357142857143"/>
+    <col customWidth="1" min="1" max="1" style="10" width="10.00390625"/>
+    <col bestFit="1" customWidth="1" min="2" max="2" style="10" width="10.005000000000001"/>
+    <col bestFit="1" customWidth="1" min="3" max="3" style="11" width="12.43357142857143"/>
+    <col bestFit="1" customWidth="1" min="4" max="4" style="12" width="10.005000000000001"/>
+    <col bestFit="1" customWidth="1" min="5" max="7" style="13" width="12.43357142857143"/>
   </cols>
   <sheetData>
     <row r="1" ht="17.25" customHeight="1">
-      <c r="A1" s="15" t="s">
+      <c r="A1" s="14" t="s">
         <v>14</v>
       </c>
-      <c r="B1" s="15" t="s">
+      <c r="B1" s="14" t="s">
         <v>15</v>
       </c>
-      <c r="C1" s="15" t="s">
+      <c r="C1" s="14" t="s">
         <v>16</v>
       </c>
-      <c r="D1" s="15" t="s">
+      <c r="D1" s="14" t="s">
         <v>17</v>
       </c>
-      <c r="E1" s="15" t="s">
+      <c r="E1" s="14" t="s">
         <v>18</v>
       </c>
-      <c r="F1" s="15" t="s">
+      <c r="F1" s="14" t="s">
         <v>19</v>
       </c>
-      <c r="G1" s="15" t="s">
+      <c r="G1" s="14" t="s">
         <v>20</v>
       </c>
     </row>
@@ -1556,22 +1561,22 @@
       <c r="A2" s="15">
         <v>0.25900000000000001</v>
       </c>
-      <c r="B2" s="15">
+      <c r="B2" s="16">
         <v>0.00080000000000000004</v>
       </c>
-      <c r="C2" s="16">
+      <c r="C2" s="17">
         <v>0.39300000000000002</v>
       </c>
-      <c r="D2" s="17">
+      <c r="D2" s="18">
         <v>0.0012999999999999999</v>
       </c>
-      <c r="E2" s="15">
+      <c r="E2" s="14">
         <v>10</v>
       </c>
-      <c r="F2" s="15">
+      <c r="F2" s="14">
         <v>253</v>
       </c>
-      <c r="G2" s="15">
+      <c r="G2" s="14">
         <v>387</v>
       </c>
     </row>
@@ -1579,171 +1584,171 @@
       <c r="A3" s="15">
         <v>0.25700000000000001</v>
       </c>
-      <c r="B3" s="15">
+      <c r="B3" s="16">
         <v>0.00059999999999999995</v>
       </c>
-      <c r="C3" s="16">
+      <c r="C3" s="17">
         <v>0.39400000000000002</v>
       </c>
-      <c r="D3" s="17">
+      <c r="D3" s="18">
         <v>0.0012999999999999999</v>
       </c>
-      <c r="E3" s="15"/>
-      <c r="F3" s="15"/>
-      <c r="G3" s="15"/>
+      <c r="E3" s="14"/>
+      <c r="F3" s="14"/>
+      <c r="G3" s="14"/>
     </row>
     <row r="4" ht="17.25" customHeight="1">
       <c r="A4" s="15">
         <v>0.25800000000000001</v>
       </c>
-      <c r="B4" s="15">
+      <c r="B4" s="16">
         <v>0.00089999999999999998</v>
       </c>
-      <c r="C4" s="16">
+      <c r="C4" s="17">
         <v>0.38900000000000001</v>
       </c>
-      <c r="D4" s="17">
+      <c r="D4" s="18">
         <v>0.0011000000000000001</v>
       </c>
-      <c r="E4" s="15"/>
-      <c r="F4" s="15"/>
-      <c r="G4" s="15"/>
+      <c r="E4" s="14"/>
+      <c r="F4" s="14"/>
+      <c r="G4" s="14"/>
     </row>
     <row r="5" ht="17.25" customHeight="1">
       <c r="A5" s="15">
         <v>0.26100000000000001</v>
       </c>
-      <c r="B5" s="15">
+      <c r="B5" s="16">
         <v>0.00069999999999999999</v>
       </c>
-      <c r="C5" s="16">
+      <c r="C5" s="17">
         <v>0.38800000000000001</v>
       </c>
-      <c r="D5" s="17">
+      <c r="D5" s="18">
         <v>0.0014</v>
       </c>
-      <c r="E5" s="15"/>
-      <c r="F5" s="15"/>
-      <c r="G5" s="15"/>
+      <c r="E5" s="14"/>
+      <c r="F5" s="14"/>
+      <c r="G5" s="14"/>
     </row>
     <row r="6" ht="17.25" customHeight="1">
       <c r="A6" s="15">
         <v>0.25900000000000001</v>
       </c>
-      <c r="B6" s="15">
+      <c r="B6" s="16">
         <v>0.00069999999999999999</v>
       </c>
-      <c r="C6" s="16">
+      <c r="C6" s="17">
         <v>0.38500000000000001</v>
       </c>
-      <c r="D6" s="17">
+      <c r="D6" s="18">
         <v>0.0011999999999999999</v>
       </c>
-      <c r="E6" s="15"/>
-      <c r="F6" s="15"/>
-      <c r="G6" s="15"/>
+      <c r="E6" s="14"/>
+      <c r="F6" s="14"/>
+      <c r="G6" s="14"/>
     </row>
     <row r="7" ht="17.25" customHeight="1">
       <c r="A7" s="15">
         <v>0.25800000000000001</v>
       </c>
-      <c r="B7" s="15">
+      <c r="B7" s="16">
         <v>0.00069999999999999999</v>
       </c>
-      <c r="C7" s="16">
+      <c r="C7" s="17">
         <v>0.38500000000000001</v>
       </c>
-      <c r="D7" s="17">
+      <c r="D7" s="18">
         <v>0.001</v>
       </c>
-      <c r="E7" s="15"/>
-      <c r="F7" s="15"/>
-      <c r="G7" s="15"/>
+      <c r="E7" s="14"/>
+      <c r="F7" s="14"/>
+      <c r="G7" s="14"/>
     </row>
     <row r="8" ht="17.25" customHeight="1">
       <c r="A8" s="15">
         <v>0.255</v>
       </c>
-      <c r="B8" s="15">
+      <c r="B8" s="16">
         <v>0.00059999999999999995</v>
       </c>
       <c r="C8" s="15">
         <v>0.38500000000000001</v>
       </c>
-      <c r="D8" s="15">
+      <c r="D8" s="16">
         <v>0.00059999999999999995</v>
       </c>
-      <c r="E8" s="15"/>
-      <c r="F8" s="15"/>
-      <c r="G8" s="15"/>
+      <c r="E8" s="14"/>
+      <c r="F8" s="14"/>
+      <c r="G8" s="14"/>
     </row>
     <row r="9" ht="17.25" customHeight="1">
       <c r="A9" s="15">
         <v>0.255</v>
       </c>
-      <c r="B9" s="15">
+      <c r="B9" s="16">
         <v>0.00069999999999999999</v>
       </c>
       <c r="C9" s="15">
         <v>0.38400000000000001</v>
       </c>
-      <c r="D9" s="15">
+      <c r="D9" s="16">
         <v>0.00080000000000000004</v>
       </c>
-      <c r="E9" s="15"/>
-      <c r="F9" s="15"/>
-      <c r="G9" s="15"/>
+      <c r="E9" s="14"/>
+      <c r="F9" s="14"/>
+      <c r="G9" s="14"/>
     </row>
     <row r="10" ht="17.25" customHeight="1">
       <c r="A10" s="15">
         <v>0.25800000000000001</v>
       </c>
-      <c r="B10" s="15">
+      <c r="B10" s="16">
         <v>0.00069999999999999999</v>
       </c>
-      <c r="C10" s="16">
+      <c r="C10" s="17">
         <v>0.39900000000000002</v>
       </c>
-      <c r="D10" s="17">
+      <c r="D10" s="18">
         <v>0.00080000000000000004</v>
       </c>
-      <c r="E10" s="15"/>
-      <c r="F10" s="15"/>
-      <c r="G10" s="15"/>
+      <c r="E10" s="14"/>
+      <c r="F10" s="14"/>
+      <c r="G10" s="14"/>
     </row>
     <row r="11" ht="17.25" customHeight="1">
       <c r="A11" s="15">
         <v>0.255</v>
       </c>
-      <c r="B11" s="15">
+      <c r="B11" s="16">
         <v>0.00050000000000000001</v>
       </c>
-      <c r="C11" s="16">
+      <c r="C11" s="17">
         <v>0.38700000000000001</v>
       </c>
-      <c r="D11" s="17">
+      <c r="D11" s="18">
         <v>0.00089999999999999998</v>
       </c>
-      <c r="E11" s="15"/>
-      <c r="F11" s="15"/>
-      <c r="G11" s="15"/>
+      <c r="E11" s="14"/>
+      <c r="F11" s="14"/>
+      <c r="G11" s="14"/>
     </row>
     <row r="12" ht="17.25" customHeight="1">
       <c r="A12" s="15">
         <v>0.25700000000000001</v>
       </c>
-      <c r="B12" s="15">
+      <c r="B12" s="16">
         <v>0.0016999999999999999</v>
       </c>
-      <c r="C12" s="16">
+      <c r="C12" s="17">
         <v>0.38500000000000001</v>
       </c>
-      <c r="D12" s="17">
+      <c r="D12" s="18">
         <v>0.00080000000000000004</v>
       </c>
-      <c r="E12" s="15"/>
-      <c r="F12" s="15"/>
-      <c r="G12" s="15"/>
+      <c r="E12" s="14"/>
+      <c r="F12" s="14"/>
+      <c r="G12" s="14"/>
     </row>
   </sheetData>
   <printOptions headings="0" gridLines="0"/>
@@ -1766,12 +1771,12 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25"/>
   <cols>
-    <col bestFit="1" customWidth="1" min="1" max="2" style="12" width="12.43357142857143"/>
+    <col bestFit="1" customWidth="1" min="1" max="2" style="11" width="12.43357142857143"/>
     <col bestFit="1" customWidth="1" min="3" max="3" style="1" width="12.43357142857143"/>
-    <col bestFit="1" customWidth="1" min="4" max="4" style="11" width="12.43357142857143"/>
-    <col bestFit="1" customWidth="1" min="5" max="5" style="18" width="12.43357142857143"/>
+    <col bestFit="1" customWidth="1" min="4" max="4" style="10" width="12.43357142857143"/>
+    <col bestFit="1" customWidth="1" min="5" max="5" style="19" width="12.43357142857143"/>
     <col bestFit="1" customWidth="1" min="6" max="7" style="1" width="12.43357142857143"/>
-    <col bestFit="1" customWidth="1" min="8" max="8" style="11" width="12.43357142857143"/>
+    <col bestFit="1" customWidth="1" min="8" max="8" style="10" width="12.43357142857143"/>
   </cols>
   <sheetData>
     <row r="1" ht="17.25" customHeight="1">
@@ -1781,19 +1786,19 @@
       <c r="B1" s="5" t="s">
         <v>22</v>
       </c>
-      <c r="C1" s="19" t="s">
+      <c r="C1" s="20" t="s">
         <v>23</v>
       </c>
       <c r="D1" s="7" t="s">
         <v>24</v>
       </c>
-      <c r="E1" s="20" t="s">
+      <c r="E1" s="21" t="s">
         <v>25</v>
       </c>
-      <c r="F1" s="19" t="s">
+      <c r="F1" s="20" t="s">
         <v>26</v>
       </c>
-      <c r="G1" s="19" t="s">
+      <c r="G1" s="20" t="s">
         <v>27</v>
       </c>
       <c r="H1" s="7" t="s">
@@ -1807,25 +1812,25 @@
       <c r="B2" s="8">
         <v>-0.27000000000000002</v>
       </c>
-      <c r="C2" s="10">
+      <c r="C2" s="22">
         <f t="shared" ref="C2:C6" si="0">$H$2*(B2-A2)</f>
         <v>-0.14025000000000001</v>
       </c>
-      <c r="D2" s="10">
+      <c r="D2" s="22">
         <v>-0.14000000000000001</v>
       </c>
-      <c r="E2" s="21">
+      <c r="E2" s="23">
         <v>0.00059999999999999995</v>
       </c>
-      <c r="F2" s="21">
+      <c r="F2" s="23">
         <f t="shared" ref="F2:F6" si="1">0.5*$H$2*B2*B2</f>
         <v>0.0092947500000000009</v>
       </c>
-      <c r="G2" s="21">
+      <c r="G2" s="23">
         <f t="shared" ref="G2:G6" si="2">F2-E2</f>
         <v>0.0086947500000000011</v>
       </c>
-      <c r="H2" s="10">
+      <c r="H2" s="22">
         <v>0.255</v>
       </c>
     </row>
@@ -1836,25 +1841,25 @@
       <c r="B3" s="8">
         <v>-0.12</v>
       </c>
-      <c r="C3" s="10">
+      <c r="C3" s="22">
         <f t="shared" si="0"/>
         <v>-0.066810000000000008</v>
       </c>
-      <c r="D3" s="10">
+      <c r="D3" s="22">
         <v>-0.059999999999999998</v>
       </c>
-      <c r="E3" s="21">
+      <c r="E3" s="23">
         <v>0.00080000000000000004</v>
       </c>
-      <c r="F3" s="21">
+      <c r="F3" s="23">
         <f t="shared" si="1"/>
         <v>0.001836</v>
       </c>
-      <c r="G3" s="21">
+      <c r="G3" s="23">
         <f t="shared" si="2"/>
         <v>0.001036</v>
       </c>
-      <c r="H3" s="22"/>
+      <c r="H3" s="24"/>
     </row>
     <row r="4" ht="17.25" customHeight="1">
       <c r="A4" s="8">
@@ -1863,26 +1868,26 @@
       <c r="B4" s="8">
         <v>-0.191</v>
       </c>
-      <c r="C4" s="10">
+      <c r="C4" s="22">
         <f t="shared" si="0"/>
         <v>-0.10149000000000001</v>
       </c>
-      <c r="D4" s="10">
+      <c r="D4" s="22">
         <v>-0.10000000000000001</v>
       </c>
-      <c r="E4" s="21">
+      <c r="E4" s="23">
         <f t="shared" ref="E4:E6" si="3">0.5*$H$2*A4*A4</f>
         <v>0.0054632474999999998</v>
       </c>
-      <c r="F4" s="21">
+      <c r="F4" s="23">
         <f t="shared" si="1"/>
         <v>0.0046513275</v>
       </c>
-      <c r="G4" s="21">
+      <c r="G4" s="23">
         <f t="shared" si="2"/>
         <v>-0.00081191999999999983</v>
       </c>
-      <c r="H4" s="22"/>
+      <c r="H4" s="24"/>
     </row>
     <row r="5" ht="17.25" customHeight="1">
       <c r="A5" s="8">
@@ -1891,26 +1896,26 @@
       <c r="B5" s="8">
         <v>-0.29199999999999998</v>
       </c>
-      <c r="C5" s="10">
+      <c r="C5" s="22">
         <f t="shared" si="0"/>
         <v>-0.15198</v>
       </c>
-      <c r="D5" s="10">
+      <c r="D5" s="22">
         <v>-0.14999999999999999</v>
       </c>
-      <c r="E5" s="21">
+      <c r="E5" s="23">
         <f t="shared" si="3"/>
         <v>0.01178304</v>
       </c>
-      <c r="F5" s="21">
+      <c r="F5" s="23">
         <f t="shared" si="1"/>
         <v>0.01087116</v>
       </c>
-      <c r="G5" s="21">
+      <c r="G5" s="23">
         <f t="shared" si="2"/>
         <v>-0.00091188000000000033</v>
       </c>
-      <c r="H5" s="22"/>
+      <c r="H5" s="24"/>
     </row>
     <row r="6" ht="17.25" customHeight="1">
       <c r="A6" s="8">
@@ -1919,86 +1924,86 @@
       <c r="B6" s="8">
         <v>-0.40500000000000003</v>
       </c>
-      <c r="C6" s="10">
+      <c r="C6" s="22">
         <f t="shared" si="0"/>
         <v>-0.20935499999999999</v>
       </c>
-      <c r="D6" s="10">
+      <c r="D6" s="22">
         <v>-0.20000000000000001</v>
       </c>
-      <c r="E6" s="21">
+      <c r="E6" s="23">
         <f t="shared" si="3"/>
         <v>0.022064639999999996</v>
       </c>
-      <c r="F6" s="21">
+      <c r="F6" s="23">
         <f t="shared" si="1"/>
         <v>0.020913187500000003</v>
       </c>
-      <c r="G6" s="21">
+      <c r="G6" s="23">
         <f t="shared" si="2"/>
         <v>-0.0011514524999999935</v>
       </c>
-      <c r="H6" s="22"/>
+      <c r="H6" s="24"/>
     </row>
     <row r="7" ht="17.25" customHeight="1">
-      <c r="A7" s="23"/>
-      <c r="B7" s="23"/>
-      <c r="C7" s="22"/>
-      <c r="D7" s="22"/>
-      <c r="E7" s="24"/>
-      <c r="F7" s="24"/>
-      <c r="G7" s="24"/>
-      <c r="H7" s="22"/>
+      <c r="A7" s="25"/>
+      <c r="B7" s="25"/>
+      <c r="C7" s="24"/>
+      <c r="D7" s="24"/>
+      <c r="E7" s="26"/>
+      <c r="F7" s="26"/>
+      <c r="G7" s="26"/>
+      <c r="H7" s="24"/>
     </row>
     <row r="8" ht="17.25" customHeight="1">
-      <c r="A8" s="23"/>
-      <c r="B8" s="23"/>
-      <c r="C8" s="22"/>
-      <c r="D8" s="22"/>
-      <c r="E8" s="24"/>
-      <c r="F8" s="24"/>
-      <c r="G8" s="24"/>
-      <c r="H8" s="22"/>
+      <c r="A8" s="25"/>
+      <c r="B8" s="25"/>
+      <c r="C8" s="24"/>
+      <c r="D8" s="24"/>
+      <c r="E8" s="26"/>
+      <c r="F8" s="26"/>
+      <c r="G8" s="26"/>
+      <c r="H8" s="24"/>
     </row>
     <row r="9" ht="17.25" customHeight="1">
-      <c r="A9" s="23"/>
-      <c r="B9" s="23"/>
-      <c r="C9" s="22"/>
-      <c r="D9" s="22"/>
-      <c r="E9" s="24"/>
-      <c r="F9" s="24"/>
-      <c r="G9" s="24"/>
-      <c r="H9" s="22"/>
+      <c r="A9" s="25"/>
+      <c r="B9" s="25"/>
+      <c r="C9" s="24"/>
+      <c r="D9" s="24"/>
+      <c r="E9" s="26"/>
+      <c r="F9" s="26"/>
+      <c r="G9" s="26"/>
+      <c r="H9" s="24"/>
     </row>
     <row r="10" ht="17.25" customHeight="1">
-      <c r="A10" s="23"/>
-      <c r="B10" s="23"/>
-      <c r="C10" s="22"/>
-      <c r="D10" s="22"/>
-      <c r="E10" s="24"/>
-      <c r="F10" s="24"/>
-      <c r="G10" s="24"/>
-      <c r="H10" s="22"/>
+      <c r="A10" s="25"/>
+      <c r="B10" s="25"/>
+      <c r="C10" s="24"/>
+      <c r="D10" s="24"/>
+      <c r="E10" s="26"/>
+      <c r="F10" s="26"/>
+      <c r="G10" s="26"/>
+      <c r="H10" s="24"/>
     </row>
     <row r="11" ht="17.25" customHeight="1">
-      <c r="A11" s="23"/>
-      <c r="B11" s="23"/>
-      <c r="C11" s="22"/>
-      <c r="D11" s="22"/>
-      <c r="E11" s="24"/>
-      <c r="F11" s="24"/>
-      <c r="G11" s="24"/>
-      <c r="H11" s="22"/>
+      <c r="A11" s="25"/>
+      <c r="B11" s="25"/>
+      <c r="C11" s="24"/>
+      <c r="D11" s="24"/>
+      <c r="E11" s="26"/>
+      <c r="F11" s="26"/>
+      <c r="G11" s="26"/>
+      <c r="H11" s="24"/>
     </row>
     <row r="12" ht="17.25" customHeight="1">
-      <c r="A12" s="23"/>
-      <c r="B12" s="23"/>
-      <c r="C12" s="22"/>
-      <c r="D12" s="22"/>
-      <c r="E12" s="24"/>
-      <c r="F12" s="24"/>
-      <c r="G12" s="24"/>
-      <c r="H12" s="22"/>
+      <c r="A12" s="25"/>
+      <c r="B12" s="25"/>
+      <c r="C12" s="24"/>
+      <c r="D12" s="24"/>
+      <c r="E12" s="26"/>
+      <c r="F12" s="26"/>
+      <c r="G12" s="26"/>
+      <c r="H12" s="24"/>
     </row>
   </sheetData>
   <printOptions headings="0" gridLines="0"/>
@@ -2022,34 +2027,34 @@
   <sheetFormatPr defaultRowHeight="14.25"/>
   <cols>
     <col bestFit="1" customWidth="1" min="1" max="2" style="2" width="12.43357142857143"/>
-    <col bestFit="1" customWidth="1" min="3" max="3" style="25" width="12.43357142857143"/>
+    <col bestFit="1" customWidth="1" min="3" max="3" style="27" width="12.43357142857143"/>
     <col bestFit="1" customWidth="1" min="4" max="4" style="4" width="12.43357142857143"/>
-    <col bestFit="1" customWidth="1" min="5" max="5" style="25" width="14.576428571428572"/>
-    <col bestFit="1" customWidth="1" min="6" max="7" style="25" width="12.43357142857143"/>
-    <col bestFit="1" customWidth="1" min="8" max="8" style="12" width="12.43357142857143"/>
+    <col bestFit="1" customWidth="1" min="5" max="5" style="27" width="14.576428571428572"/>
+    <col bestFit="1" customWidth="1" min="6" max="7" style="27" width="12.43357142857143"/>
+    <col bestFit="1" customWidth="1" min="8" max="8" style="11" width="12.43357142857143"/>
     <col bestFit="1" customWidth="1" min="9" max="9" style="1" width="12.43357142857143"/>
   </cols>
   <sheetData>
     <row r="1" ht="17.25" customHeight="1">
-      <c r="A1" s="23" t="s">
+      <c r="A1" s="25" t="s">
         <v>29</v>
       </c>
-      <c r="B1" s="23" t="s">
+      <c r="B1" s="25" t="s">
         <v>22</v>
       </c>
-      <c r="C1" s="26" t="s">
+      <c r="C1" s="28" t="s">
         <v>23</v>
       </c>
-      <c r="D1" s="22" t="s">
+      <c r="D1" s="24" t="s">
         <v>24</v>
       </c>
-      <c r="E1" s="26" t="s">
+      <c r="E1" s="28" t="s">
         <v>25</v>
       </c>
-      <c r="F1" s="26" t="s">
+      <c r="F1" s="28" t="s">
         <v>26</v>
       </c>
-      <c r="G1" s="26" t="s">
+      <c r="G1" s="28" t="s">
         <v>27</v>
       </c>
       <c r="H1" s="5" t="s">
@@ -2064,29 +2069,29 @@
       <c r="B2" s="8">
         <v>-0.309</v>
       </c>
-      <c r="C2" s="10">
+      <c r="C2" s="22">
         <f t="shared" ref="C2:C9" si="4">$H$2*(-A2+B2)</f>
         <v>-0.17172000000000001</v>
       </c>
-      <c r="D2" s="10">
+      <c r="D2" s="22">
         <v>-0.14000000000000001</v>
       </c>
-      <c r="E2" s="21">
+      <c r="E2" s="23">
         <f t="shared" ref="E2:E9" si="5">0.5*$H$2*A2*A2</f>
         <v>0.014435415000000002</v>
       </c>
-      <c r="F2" s="21">
+      <c r="F2" s="23">
         <f t="shared" ref="F2:F9" si="6">0.5*$H$2*B2*B2</f>
         <v>0.012889935</v>
       </c>
-      <c r="G2" s="21">
+      <c r="G2" s="23">
         <f t="shared" ref="G2:G9" si="7">F2-E2</f>
         <v>-0.0015454800000000019</v>
       </c>
       <c r="H2" s="8">
         <v>0.27000000000000002</v>
       </c>
-      <c r="I2" s="21"/>
+      <c r="I2" s="23"/>
     </row>
     <row r="3" ht="17.25" customHeight="1">
       <c r="A3" s="8">
@@ -2095,26 +2100,26 @@
       <c r="B3" s="8">
         <v>-0.35899999999999999</v>
       </c>
-      <c r="C3" s="10">
+      <c r="C3" s="22">
         <f t="shared" si="4"/>
         <v>-0.19683</v>
       </c>
-      <c r="D3" s="10">
+      <c r="D3" s="22">
         <v>-0.14999999999999999</v>
       </c>
-      <c r="E3" s="21">
+      <c r="E3" s="23">
         <f t="shared" si="5"/>
         <v>0.018481500000000001</v>
       </c>
-      <c r="F3" s="21">
+      <c r="F3" s="23">
         <f t="shared" si="6"/>
         <v>0.017398935000000001</v>
       </c>
-      <c r="G3" s="21">
+      <c r="G3" s="23">
         <f t="shared" si="7"/>
         <v>-0.0010825650000000006</v>
       </c>
-      <c r="H3" s="23"/>
+      <c r="H3" s="25"/>
       <c r="I3" s="1"/>
     </row>
     <row r="4" ht="17.25" customHeight="1">
@@ -2124,26 +2129,26 @@
       <c r="B4" s="8">
         <v>-0.248</v>
       </c>
-      <c r="C4" s="10">
+      <c r="C4" s="22">
         <f t="shared" si="4"/>
         <v>-0.13689000000000001</v>
       </c>
-      <c r="D4" s="10">
+      <c r="D4" s="22">
         <v>-0.14999999999999999</v>
       </c>
-      <c r="E4" s="21">
+      <c r="E4" s="23">
         <f t="shared" si="5"/>
         <v>0.0090559350000000011</v>
       </c>
-      <c r="F4" s="21">
+      <c r="F4" s="23">
         <f t="shared" si="6"/>
         <v>0.0083030400000000011</v>
       </c>
-      <c r="G4" s="21">
+      <c r="G4" s="23">
         <f t="shared" si="7"/>
         <v>-0.00075289499999999995</v>
       </c>
-      <c r="H4" s="23"/>
+      <c r="H4" s="25"/>
       <c r="I4" s="1"/>
     </row>
     <row r="5" ht="17.25" customHeight="1">
@@ -2153,26 +2158,26 @@
       <c r="B5" s="8">
         <v>-0.35599999999999998</v>
       </c>
-      <c r="C5" s="10">
+      <c r="C5" s="22">
         <f t="shared" si="4"/>
         <v>-0.19440000000000002</v>
       </c>
-      <c r="D5" s="10">
+      <c r="D5" s="22">
         <v>-0.14999999999999999</v>
       </c>
-      <c r="E5" s="21">
+      <c r="E5" s="23">
         <f t="shared" si="5"/>
         <v>0.01788696</v>
       </c>
-      <c r="F5" s="21">
+      <c r="F5" s="23">
         <f t="shared" si="6"/>
         <v>0.017109359999999997</v>
       </c>
-      <c r="G5" s="21">
+      <c r="G5" s="23">
         <f t="shared" si="7"/>
         <v>-0.00077760000000000329</v>
       </c>
-      <c r="H5" s="23"/>
+      <c r="H5" s="25"/>
       <c r="I5" s="1"/>
     </row>
     <row r="6" ht="17.25" customHeight="1">
@@ -2182,26 +2187,26 @@
       <c r="B6" s="8">
         <v>-0.29499999999999998</v>
       </c>
-      <c r="C6" s="10">
+      <c r="C6" s="22">
         <f t="shared" si="4"/>
         <v>-0.16281000000000001</v>
       </c>
-      <c r="D6" s="10">
+      <c r="D6" s="22">
         <v>-0.14000000000000001</v>
       </c>
-      <c r="E6" s="21">
+      <c r="E6" s="23">
         <f t="shared" si="5"/>
         <v>0.012806639999999999</v>
       </c>
-      <c r="F6" s="21">
+      <c r="F6" s="23">
         <f t="shared" si="6"/>
         <v>0.011748374999999998</v>
       </c>
-      <c r="G6" s="21">
+      <c r="G6" s="23">
         <f t="shared" si="7"/>
         <v>-0.0010582650000000009</v>
       </c>
-      <c r="H6" s="23"/>
+      <c r="H6" s="25"/>
       <c r="I6" s="1"/>
     </row>
     <row r="7" ht="17.25" customHeight="1">
@@ -2211,26 +2216,26 @@
       <c r="B7" s="8">
         <v>-0.38700000000000001</v>
       </c>
-      <c r="C7" s="10">
+      <c r="C7" s="22">
         <f t="shared" si="4"/>
         <v>-0.21060000000000001</v>
       </c>
-      <c r="D7" s="10">
+      <c r="D7" s="22">
         <v>-0.17000000000000001</v>
       </c>
-      <c r="E7" s="21">
+      <c r="E7" s="23">
         <f t="shared" si="5"/>
         <v>0.020850615000000003</v>
       </c>
-      <c r="F7" s="21">
+      <c r="F7" s="23">
         <f t="shared" si="6"/>
         <v>0.020218815000000005</v>
       </c>
-      <c r="G7" s="21">
+      <c r="G7" s="23">
         <f t="shared" si="7"/>
         <v>-0.00063179999999999834</v>
       </c>
-      <c r="H7" s="23"/>
+      <c r="H7" s="25"/>
       <c r="I7" s="1"/>
     </row>
     <row r="8" ht="17.25" customHeight="1">
@@ -2240,26 +2245,26 @@
       <c r="B8" s="8">
         <v>-0.502</v>
       </c>
-      <c r="C8" s="10">
+      <c r="C8" s="22">
         <f t="shared" si="4"/>
         <v>-0.27134999999999998</v>
       </c>
-      <c r="D8" s="10">
+      <c r="D8" s="22">
         <v>-0.23999999999999999</v>
       </c>
-      <c r="E8" s="21">
+      <c r="E8" s="23">
         <f t="shared" si="5"/>
         <v>0.034156215000000004</v>
       </c>
-      <c r="F8" s="21">
+      <c r="F8" s="23">
         <f t="shared" si="6"/>
         <v>0.034020540000000009</v>
       </c>
-      <c r="G8" s="21">
+      <c r="G8" s="23">
         <f t="shared" si="7"/>
         <v>-0.00013567499999999483</v>
       </c>
-      <c r="H8" s="23"/>
+      <c r="H8" s="25"/>
       <c r="I8" s="1"/>
     </row>
     <row r="9" ht="17.25" customHeight="1">
@@ -2269,26 +2274,26 @@
       <c r="B9" s="8">
         <v>-0.45700000000000002</v>
       </c>
-      <c r="C9" s="10">
+      <c r="C9" s="22">
         <f t="shared" si="4"/>
         <v>-0.25191000000000002</v>
       </c>
-      <c r="D9" s="10">
+      <c r="D9" s="22">
         <v>-0.27000000000000002</v>
       </c>
-      <c r="E9" s="21">
+      <c r="E9" s="23">
         <f t="shared" si="5"/>
         <v>0.030587759999999999</v>
       </c>
-      <c r="F9" s="21">
+      <c r="F9" s="23">
         <f t="shared" si="6"/>
         <v>0.028194615000000003</v>
       </c>
-      <c r="G9" s="21">
+      <c r="G9" s="23">
         <f t="shared" si="7"/>
         <v>-0.0023931449999999958</v>
       </c>
-      <c r="H9" s="23"/>
+      <c r="H9" s="25"/>
       <c r="I9" s="1"/>
     </row>
     <row r="10" ht="17.25" customHeight="1">
@@ -2298,26 +2303,26 @@
       <c r="B10" s="8">
         <v>-0.312</v>
       </c>
-      <c r="C10" s="10">
+      <c r="C10" s="22">
         <f t="shared" ref="C10:C12" si="8">$H$2*(-A10+B10)</f>
         <v>-0.16875000000000001</v>
       </c>
-      <c r="D10" s="10">
+      <c r="D10" s="22">
         <v>-0.16</v>
       </c>
-      <c r="E10" s="21">
+      <c r="E10" s="23">
         <f t="shared" ref="E10:E12" si="9">0.5*$H$2*A10*A10</f>
         <v>0.013225815</v>
       </c>
-      <c r="F10" s="21">
+      <c r="F10" s="23">
         <f t="shared" ref="F10:F12" si="10">0.5*$H$2*B10*B10</f>
         <v>0.013141440000000001</v>
       </c>
-      <c r="G10" s="21">
+      <c r="G10" s="23">
         <f t="shared" ref="G10:G12" si="11">F10-E10</f>
         <v>-8.4374999999999381e-05</v>
       </c>
-      <c r="H10" s="23"/>
+      <c r="H10" s="25"/>
       <c r="I10" s="1"/>
     </row>
     <row r="11" ht="17.25" customHeight="1">
@@ -2327,26 +2332,26 @@
       <c r="B11" s="8">
         <v>-0.439</v>
       </c>
-      <c r="C11" s="10">
+      <c r="C11" s="22">
         <f t="shared" si="8"/>
         <v>-0.23733000000000001</v>
       </c>
-      <c r="D11" s="10">
+      <c r="D11" s="22">
         <v>-0.22</v>
       </c>
-      <c r="E11" s="21">
+      <c r="E11" s="23">
         <f t="shared" si="9"/>
         <v>0.026136</v>
       </c>
-      <c r="F11" s="21">
+      <c r="F11" s="23">
         <f t="shared" si="10"/>
         <v>0.026017335000000003</v>
       </c>
-      <c r="G11" s="21">
+      <c r="G11" s="23">
         <f t="shared" si="11"/>
         <v>-0.00011866499999999697</v>
       </c>
-      <c r="H11" s="23"/>
+      <c r="H11" s="25"/>
       <c r="I11" s="1"/>
     </row>
     <row r="12" ht="17.25" customHeight="1">
@@ -2356,26 +2361,26 @@
       <c r="B12" s="8">
         <v>-0.312</v>
       </c>
-      <c r="C12" s="10">
+      <c r="C12" s="22">
         <f t="shared" si="8"/>
         <v>-0.17388000000000001</v>
       </c>
-      <c r="D12" s="10">
+      <c r="D12" s="22">
         <v>-0.20000000000000001</v>
       </c>
-      <c r="E12" s="21">
+      <c r="E12" s="23">
         <f t="shared" si="9"/>
         <v>0.014880240000000003</v>
       </c>
-      <c r="F12" s="21">
+      <c r="F12" s="23">
         <f t="shared" si="10"/>
         <v>0.013141440000000001</v>
       </c>
-      <c r="G12" s="21">
+      <c r="G12" s="23">
         <f t="shared" si="11"/>
         <v>-0.0017388000000000021</v>
       </c>
-      <c r="H12" s="23"/>
+      <c r="H12" s="25"/>
       <c r="I12" s="1"/>
     </row>
   </sheetData>
@@ -2399,7 +2404,7 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25"/>
   <cols>
-    <col bestFit="1" customWidth="1" min="1" max="4" style="12" width="12.43357142857143"/>
+    <col bestFit="1" customWidth="1" min="1" max="4" style="11" width="12.43357142857143"/>
     <col bestFit="1" customWidth="1" min="5" max="10" style="1" width="12.43357142857143"/>
   </cols>
   <sheetData>
@@ -2416,22 +2421,22 @@
       <c r="D1" s="5" t="s">
         <v>33</v>
       </c>
-      <c r="E1" s="19" t="s">
+      <c r="E1" s="20" t="s">
         <v>25</v>
       </c>
-      <c r="F1" s="19" t="s">
+      <c r="F1" s="20" t="s">
         <v>26</v>
       </c>
-      <c r="G1" s="19" t="s">
+      <c r="G1" s="20" t="s">
         <v>27</v>
       </c>
-      <c r="H1" s="19" t="s">
+      <c r="H1" s="20" t="s">
         <v>34</v>
       </c>
-      <c r="I1" s="19" t="s">
+      <c r="I1" s="20" t="s">
         <v>35</v>
       </c>
-      <c r="J1" s="19" t="s">
+      <c r="J1" s="20" t="s">
         <v>23</v>
       </c>
     </row>
@@ -2448,11 +2453,11 @@
       <c r="D2" s="8">
         <v>0.27000000000000002</v>
       </c>
-      <c r="E2" s="21">
+      <c r="E2" s="23">
         <f t="shared" ref="E2:E9" si="12">0.5*($D$2)*B2*B2</f>
         <v>0.029316060000000005</v>
       </c>
-      <c r="F2" s="21">
+      <c r="F2" s="23">
         <f t="shared" ref="F2:F9" si="13">0.5*$C$2*A2*A2</f>
         <v>0.027518536500000003</v>
       </c>
@@ -2460,11 +2465,11 @@
         <f t="shared" ref="G2:G9" si="14">F2-E2</f>
         <v>-0.001797523500000002</v>
       </c>
-      <c r="H2" s="21">
+      <c r="H2" s="23">
         <f t="shared" ref="H2:H9" si="15">$D$2*B2</f>
         <v>0.12582000000000002</v>
       </c>
-      <c r="I2" s="21">
+      <c r="I2" s="23">
         <f t="shared" ref="I2:I9" si="16">$C$2*A2</f>
         <v>0.12257700000000001</v>
       </c>
@@ -2480,13 +2485,13 @@
       <c r="B3" s="8">
         <v>0.65800000000000003</v>
       </c>
-      <c r="C3" s="23"/>
-      <c r="D3" s="23"/>
-      <c r="E3" s="21">
+      <c r="C3" s="25"/>
+      <c r="D3" s="25"/>
+      <c r="E3" s="23">
         <f t="shared" si="12"/>
         <v>0.058450140000000005</v>
       </c>
-      <c r="F3" s="21">
+      <c r="F3" s="23">
         <f t="shared" si="13"/>
         <v>0.054176849999999999</v>
       </c>
@@ -2494,11 +2499,11 @@
         <f t="shared" si="14"/>
         <v>-0.004273290000000006</v>
       </c>
-      <c r="H3" s="21">
+      <c r="H3" s="23">
         <f t="shared" si="15"/>
         <v>0.17766000000000001</v>
       </c>
-      <c r="I3" s="21">
+      <c r="I3" s="23">
         <f t="shared" si="16"/>
         <v>0.17199</v>
       </c>
@@ -2514,13 +2519,13 @@
       <c r="B4" s="8">
         <v>0.64800000000000002</v>
       </c>
-      <c r="C4" s="23"/>
-      <c r="D4" s="23"/>
-      <c r="E4" s="21">
+      <c r="C4" s="25"/>
+      <c r="D4" s="25"/>
+      <c r="E4" s="23">
         <f t="shared" si="12"/>
         <v>0.056687040000000001</v>
       </c>
-      <c r="F4" s="21">
+      <c r="F4" s="23">
         <f t="shared" si="13"/>
         <v>0.053149823999999998</v>
       </c>
@@ -2528,11 +2533,11 @@
         <f t="shared" si="14"/>
         <v>-0.0035372160000000027</v>
       </c>
-      <c r="H4" s="21">
+      <c r="H4" s="23">
         <f t="shared" si="15"/>
         <v>0.17496</v>
       </c>
-      <c r="I4" s="21">
+      <c r="I4" s="23">
         <f t="shared" si="16"/>
         <v>0.170352</v>
       </c>
@@ -2548,13 +2553,13 @@
       <c r="B5" s="8">
         <v>0.59399999999999997</v>
       </c>
-      <c r="C5" s="23"/>
-      <c r="D5" s="23"/>
-      <c r="E5" s="21">
+      <c r="C5" s="25"/>
+      <c r="D5" s="25"/>
+      <c r="E5" s="23">
         <f t="shared" si="12"/>
         <v>0.047632859999999999</v>
       </c>
-      <c r="F5" s="21">
+      <c r="F5" s="23">
         <f t="shared" si="13"/>
         <v>0.044348849999999995</v>
       </c>
@@ -2562,11 +2567,11 @@
         <f t="shared" si="14"/>
         <v>-0.0032840100000000039</v>
       </c>
-      <c r="H5" s="21">
+      <c r="H5" s="23">
         <f t="shared" si="15"/>
         <v>0.16037999999999999</v>
       </c>
-      <c r="I5" s="21">
+      <c r="I5" s="23">
         <f t="shared" si="16"/>
         <v>0.15561</v>
       </c>
@@ -2582,13 +2587,13 @@
       <c r="B6" s="8">
         <v>0.60899999999999999</v>
       </c>
-      <c r="C6" s="23"/>
-      <c r="D6" s="23"/>
-      <c r="E6" s="21">
+      <c r="C6" s="25"/>
+      <c r="D6" s="25"/>
+      <c r="E6" s="23">
         <f t="shared" si="12"/>
         <v>0.050068935000000002</v>
       </c>
-      <c r="F6" s="21">
+      <c r="F6" s="23">
         <f t="shared" si="13"/>
         <v>0.047194055999999998</v>
       </c>
@@ -2596,11 +2601,11 @@
         <f t="shared" si="14"/>
         <v>-0.0028748790000000038</v>
       </c>
-      <c r="H6" s="21">
+      <c r="H6" s="23">
         <f t="shared" si="15"/>
         <v>0.16443000000000002</v>
       </c>
-      <c r="I6" s="21">
+      <c r="I6" s="23">
         <f t="shared" si="16"/>
         <v>0.160524</v>
       </c>
@@ -2616,13 +2621,13 @@
       <c r="B7" s="8">
         <v>0.83699999999999997</v>
       </c>
-      <c r="C7" s="23"/>
-      <c r="D7" s="23"/>
-      <c r="E7" s="21">
+      <c r="C7" s="25"/>
+      <c r="D7" s="25"/>
+      <c r="E7" s="23">
         <f t="shared" si="12"/>
         <v>0.094576814999999995</v>
       </c>
-      <c r="F7" s="21">
+      <c r="F7" s="23">
         <f t="shared" si="13"/>
         <v>0.089336656500000014</v>
       </c>
@@ -2630,11 +2635,11 @@
         <f t="shared" si="14"/>
         <v>-0.0052401584999999806</v>
       </c>
-      <c r="H7" s="21">
+      <c r="H7" s="23">
         <f t="shared" si="15"/>
         <v>0.22599</v>
       </c>
-      <c r="I7" s="21">
+      <c r="I7" s="23">
         <f t="shared" si="16"/>
         <v>0.22085700000000003</v>
       </c>
@@ -2650,13 +2655,13 @@
       <c r="B8" s="8">
         <v>0.878</v>
       </c>
-      <c r="C8" s="23"/>
-      <c r="D8" s="23"/>
-      <c r="E8" s="21">
+      <c r="C8" s="25"/>
+      <c r="D8" s="25"/>
+      <c r="E8" s="23">
         <f t="shared" si="12"/>
         <v>0.10406934000000001</v>
       </c>
-      <c r="F8" s="21">
+      <c r="F8" s="23">
         <f t="shared" si="13"/>
         <v>0.1016609685</v>
       </c>
@@ -2664,11 +2669,11 @@
         <f t="shared" si="14"/>
         <v>-0.0024083715000000061</v>
       </c>
-      <c r="H8" s="21">
+      <c r="H8" s="23">
         <f t="shared" si="15"/>
         <v>0.23706000000000002</v>
       </c>
-      <c r="I8" s="21">
+      <c r="I8" s="23">
         <f t="shared" si="16"/>
         <v>0.235599</v>
       </c>
@@ -2684,13 +2689,13 @@
       <c r="B9" s="8">
         <v>0.69099999999999995</v>
       </c>
-      <c r="C9" s="23"/>
-      <c r="D9" s="23"/>
-      <c r="E9" s="21">
+      <c r="C9" s="25"/>
+      <c r="D9" s="25"/>
+      <c r="E9" s="23">
         <f t="shared" si="12"/>
         <v>0.064459934999999996</v>
       </c>
-      <c r="F9" s="21">
+      <c r="F9" s="23">
         <f t="shared" si="13"/>
         <v>0.060001168500000007</v>
       </c>
@@ -2698,11 +2703,11 @@
         <f t="shared" si="14"/>
         <v>-0.0044587664999999888</v>
       </c>
-      <c r="H9" s="21">
+      <c r="H9" s="23">
         <f t="shared" si="15"/>
         <v>0.18656999999999999</v>
       </c>
-      <c r="I9" s="21">
+      <c r="I9" s="23">
         <f t="shared" si="16"/>
         <v>0.18099900000000002</v>
       </c>
@@ -2714,26 +2719,26 @@
     <row r="10" ht="17.25" customHeight="1">
       <c r="A10" s="8"/>
       <c r="B10" s="8"/>
-      <c r="C10" s="23"/>
-      <c r="D10" s="23"/>
-      <c r="E10" s="24"/>
-      <c r="F10" s="24"/>
-      <c r="G10" s="23"/>
-      <c r="H10" s="24"/>
-      <c r="I10" s="24"/>
-      <c r="J10" s="23"/>
+      <c r="C10" s="25"/>
+      <c r="D10" s="25"/>
+      <c r="E10" s="26"/>
+      <c r="F10" s="26"/>
+      <c r="G10" s="25"/>
+      <c r="H10" s="26"/>
+      <c r="I10" s="26"/>
+      <c r="J10" s="25"/>
     </row>
     <row r="11" ht="17.25" customHeight="1">
-      <c r="A11" s="23"/>
-      <c r="B11" s="23"/>
-      <c r="C11" s="23"/>
-      <c r="D11" s="23"/>
-      <c r="E11" s="24"/>
-      <c r="F11" s="24"/>
-      <c r="G11" s="23"/>
-      <c r="H11" s="24"/>
-      <c r="I11" s="24"/>
-      <c r="J11" s="23"/>
+      <c r="A11" s="25"/>
+      <c r="B11" s="25"/>
+      <c r="C11" s="25"/>
+      <c r="D11" s="25"/>
+      <c r="E11" s="26"/>
+      <c r="F11" s="26"/>
+      <c r="G11" s="25"/>
+      <c r="H11" s="26"/>
+      <c r="I11" s="26"/>
+      <c r="J11" s="25"/>
     </row>
   </sheetData>
   <printOptions headings="0" gridLines="0"/>
@@ -2757,16 +2762,16 @@
   <sheetFormatPr defaultRowHeight="14.25"/>
   <cols>
     <col bestFit="1" customWidth="1" min="1" max="2" style="2" width="12.43357142857143"/>
-    <col bestFit="1" customWidth="1" min="3" max="4" style="12" width="12.43357142857143"/>
-    <col bestFit="1" customWidth="1" min="5" max="5" style="14" width="12.43357142857143"/>
-    <col bestFit="1" customWidth="1" min="6" max="13" style="25" width="12.43357142857143"/>
+    <col bestFit="1" customWidth="1" min="3" max="4" style="11" width="12.43357142857143"/>
+    <col bestFit="1" customWidth="1" min="5" max="5" style="13" width="12.43357142857143"/>
+    <col bestFit="1" customWidth="1" min="6" max="13" style="27" width="12.43357142857143"/>
   </cols>
   <sheetData>
     <row r="1" ht="17.25" customHeight="1">
-      <c r="A1" s="23" t="s">
+      <c r="A1" s="25" t="s">
         <v>36</v>
       </c>
-      <c r="B1" s="23" t="s">
+      <c r="B1" s="25" t="s">
         <v>37</v>
       </c>
       <c r="C1" s="5" t="s">
@@ -2775,31 +2780,31 @@
       <c r="D1" s="5" t="s">
         <v>39</v>
       </c>
-      <c r="E1" s="27" t="s">
+      <c r="E1" s="29" t="s">
         <v>40</v>
       </c>
-      <c r="F1" s="26" t="s">
+      <c r="F1" s="28" t="s">
         <v>25</v>
       </c>
-      <c r="G1" s="26" t="s">
+      <c r="G1" s="28" t="s">
         <v>26</v>
       </c>
-      <c r="H1" s="26" t="s">
+      <c r="H1" s="28" t="s">
         <v>27</v>
       </c>
-      <c r="I1" s="26" t="s">
+      <c r="I1" s="28" t="s">
         <v>41</v>
       </c>
-      <c r="J1" s="26" t="s">
+      <c r="J1" s="28" t="s">
         <v>42</v>
       </c>
-      <c r="K1" s="26" t="s">
+      <c r="K1" s="28" t="s">
         <v>34</v>
       </c>
-      <c r="L1" s="26" t="s">
+      <c r="L1" s="28" t="s">
         <v>35</v>
       </c>
-      <c r="M1" s="26" t="s">
+      <c r="M1" s="28" t="s">
         <v>23</v>
       </c>
     </row>
@@ -2816,14 +2821,14 @@
       <c r="D2" s="8">
         <v>0.247</v>
       </c>
-      <c r="E2" s="28">
+      <c r="E2" s="30">
         <v>0</v>
       </c>
-      <c r="F2" s="21">
+      <c r="F2" s="23">
         <f t="shared" ref="F2:F9" si="18">0.5*$D$2*A2*A2</f>
         <v>0.016907149999999999</v>
       </c>
-      <c r="G2" s="21">
+      <c r="G2" s="23">
         <f t="shared" ref="G2:G9" si="19">0.5*($C$2+$D$2)*B2*B2</f>
         <v>0.0078734739999999984</v>
       </c>
@@ -2835,7 +2840,7 @@
         <f t="shared" ref="I2:I9" si="21">B2-A2</f>
         <v>0.192</v>
       </c>
-      <c r="J2" s="29">
+      <c r="J2" s="31">
         <f t="shared" ref="J2:J9" si="22">I2/A2</f>
         <v>-0.51891891891891895</v>
       </c>
@@ -2859,14 +2864,14 @@
       <c r="B3" s="8">
         <v>-0.24299999999999999</v>
       </c>
-      <c r="C3" s="23"/>
-      <c r="D3" s="23"/>
-      <c r="E3" s="30"/>
-      <c r="F3" s="21">
+      <c r="C3" s="25"/>
+      <c r="D3" s="25"/>
+      <c r="E3" s="32"/>
+      <c r="F3" s="23">
         <f t="shared" si="18"/>
         <v>0.031122493999999997</v>
       </c>
-      <c r="G3" s="21">
+      <c r="G3" s="23">
         <f t="shared" si="19"/>
         <v>0.014673676499999998</v>
       </c>
@@ -2878,7 +2883,7 @@
         <f t="shared" si="21"/>
         <v>0.25900000000000001</v>
       </c>
-      <c r="J3" s="29">
+      <c r="J3" s="31">
         <f t="shared" si="22"/>
         <v>-0.51593625498007967</v>
       </c>
@@ -2902,14 +2907,14 @@
       <c r="B4" s="8">
         <v>-0.30199999999999999</v>
       </c>
-      <c r="C4" s="23"/>
-      <c r="D4" s="23"/>
-      <c r="E4" s="30"/>
-      <c r="F4" s="21">
+      <c r="C4" s="25"/>
+      <c r="D4" s="25"/>
+      <c r="E4" s="32"/>
+      <c r="F4" s="23">
         <f t="shared" si="18"/>
         <v>0.046710787499999996</v>
       </c>
-      <c r="G4" s="21">
+      <c r="G4" s="23">
         <f t="shared" si="19"/>
         <v>0.022664193999999999</v>
       </c>
@@ -2921,7 +2926,7 @@
         <f t="shared" si="21"/>
         <v>0.313</v>
       </c>
-      <c r="J4" s="29">
+      <c r="J4" s="31">
         <f t="shared" si="22"/>
         <v>-0.50894308943089428</v>
       </c>
@@ -2945,14 +2950,14 @@
       <c r="B5" s="8">
         <v>-0.32000000000000001</v>
       </c>
-      <c r="C5" s="23"/>
-      <c r="D5" s="23"/>
-      <c r="E5" s="30"/>
-      <c r="F5" s="21">
+      <c r="C5" s="25"/>
+      <c r="D5" s="25"/>
+      <c r="E5" s="32"/>
+      <c r="F5" s="23">
         <f t="shared" si="18"/>
         <v>0.053146496000000008</v>
       </c>
-      <c r="G5" s="21">
+      <c r="G5" s="23">
         <f t="shared" si="19"/>
         <v>0.025446400000000004</v>
       </c>
@@ -2964,7 +2969,7 @@
         <f t="shared" si="21"/>
         <v>0.33600000000000002</v>
       </c>
-      <c r="J5" s="29">
+      <c r="J5" s="31">
         <f t="shared" si="22"/>
         <v>-0.51219512195121952</v>
       </c>
@@ -2988,14 +2993,14 @@
       <c r="B6" s="8">
         <v>-0.26400000000000001</v>
       </c>
-      <c r="C6" s="23"/>
-      <c r="D6" s="23"/>
-      <c r="E6" s="30"/>
-      <c r="F6" s="21">
+      <c r="C6" s="25"/>
+      <c r="D6" s="25"/>
+      <c r="E6" s="32"/>
+      <c r="F6" s="23">
         <f t="shared" si="18"/>
         <v>0.036952311500000001</v>
       </c>
-      <c r="G6" s="21">
+      <c r="G6" s="23">
         <f t="shared" si="19"/>
         <v>0.017319456000000004</v>
       </c>
@@ -3007,7 +3012,7 @@
         <f t="shared" si="21"/>
         <v>0.28300000000000003</v>
       </c>
-      <c r="J6" s="29">
+      <c r="J6" s="31">
         <f t="shared" si="22"/>
         <v>-0.51736745886654478</v>
       </c>
@@ -3031,14 +3036,14 @@
       <c r="B7" s="8">
         <v>-0.33000000000000002</v>
       </c>
-      <c r="C7" s="23"/>
-      <c r="D7" s="23"/>
-      <c r="E7" s="30"/>
-      <c r="F7" s="21">
+      <c r="C7" s="25"/>
+      <c r="D7" s="25"/>
+      <c r="E7" s="32"/>
+      <c r="F7" s="23">
         <f t="shared" si="18"/>
         <v>0.056938563500000004</v>
       </c>
-      <c r="G7" s="21">
+      <c r="G7" s="23">
         <f t="shared" si="19"/>
         <v>0.027061650000000003</v>
       </c>
@@ -3050,7 +3055,7 @@
         <f t="shared" si="21"/>
         <v>0.34900000000000003</v>
       </c>
-      <c r="J7" s="29">
+      <c r="J7" s="31">
         <f t="shared" si="22"/>
         <v>-0.51399116347569962</v>
       </c>
@@ -3074,14 +3079,14 @@
       <c r="B8" s="8">
         <v>-0.26900000000000002</v>
       </c>
-      <c r="C8" s="23"/>
-      <c r="D8" s="23"/>
-      <c r="E8" s="30"/>
-      <c r="F8" s="21">
+      <c r="C8" s="25"/>
+      <c r="D8" s="25"/>
+      <c r="E8" s="32"/>
+      <c r="F8" s="23">
         <f t="shared" si="18"/>
         <v>0.038178296000000007</v>
       </c>
-      <c r="G8" s="21">
+      <c r="G8" s="23">
         <f t="shared" si="19"/>
         <v>0.017981708500000002</v>
       </c>
@@ -3093,7 +3098,7 @@
         <f t="shared" si="21"/>
         <v>0.28700000000000003</v>
       </c>
-      <c r="J8" s="29">
+      <c r="J8" s="31">
         <f t="shared" si="22"/>
         <v>-0.51618705035971224</v>
       </c>
@@ -3117,14 +3122,14 @@
       <c r="B9" s="8">
         <v>-0.26000000000000001</v>
       </c>
-      <c r="C9" s="23"/>
-      <c r="D9" s="23"/>
-      <c r="E9" s="30"/>
-      <c r="F9" s="21">
+      <c r="C9" s="25"/>
+      <c r="D9" s="25"/>
+      <c r="E9" s="32"/>
+      <c r="F9" s="23">
         <f t="shared" si="18"/>
         <v>0.035348787500000006</v>
       </c>
-      <c r="G9" s="21">
+      <c r="G9" s="23">
         <f t="shared" si="19"/>
         <v>0.0167986</v>
       </c>
@@ -3136,7 +3141,7 @@
         <f t="shared" si="21"/>
         <v>0.27500000000000002</v>
       </c>
-      <c r="J9" s="29">
+      <c r="J9" s="31">
         <f t="shared" si="22"/>
         <v>-0.5140186915887851</v>
       </c>
@@ -3160,14 +3165,14 @@
       <c r="B10" s="8">
         <v>-0.27000000000000002</v>
       </c>
-      <c r="C10" s="23"/>
-      <c r="D10" s="23"/>
-      <c r="E10" s="30"/>
-      <c r="F10" s="21">
+      <c r="C10" s="25"/>
+      <c r="D10" s="25"/>
+      <c r="E10" s="32"/>
+      <c r="F10" s="23">
         <f>0.5*$D$2*A10*A10</f>
         <v>0.038178296000000007</v>
       </c>
-      <c r="G10" s="21">
+      <c r="G10" s="23">
         <f>0.5*($C$2+$D$2)*B10*B10</f>
         <v>0.018115650000000001</v>
       </c>
@@ -3179,7 +3184,7 @@
         <f>B10-A10</f>
         <v>0.28600000000000003</v>
       </c>
-      <c r="J10" s="29">
+      <c r="J10" s="31">
         <f>I10/A10</f>
         <v>-0.51438848920863312</v>
       </c>
@@ -3219,14 +3224,14 @@
   <cols>
     <col bestFit="1" customWidth="1" min="1" max="2" style="4" width="12.43357142857143"/>
     <col bestFit="1" customWidth="1" min="3" max="8" style="1" width="12.43357142857143"/>
-    <col bestFit="1" customWidth="1" min="9" max="10" style="12" width="12.43357142857143"/>
+    <col bestFit="1" customWidth="1" min="9" max="10" style="11" width="12.43357142857143"/>
   </cols>
   <sheetData>
     <row r="1" ht="17.25" customHeight="1">
-      <c r="A1" s="22" t="s">
+      <c r="A1" s="24" t="s">
         <v>31</v>
       </c>
-      <c r="B1" s="22" t="s">
+      <c r="B1" s="24" t="s">
         <v>22</v>
       </c>
       <c r="C1" s="1"/>
@@ -3275,8 +3280,8 @@
       <c r="F3" s="1"/>
       <c r="G3" s="1"/>
       <c r="H3" s="1"/>
-      <c r="I3" s="23"/>
-      <c r="J3" s="23"/>
+      <c r="I3" s="25"/>
+      <c r="J3" s="25"/>
     </row>
     <row r="4" ht="17.25" customHeight="1">
       <c r="A4" s="8">
@@ -3291,8 +3296,8 @@
       <c r="F4" s="1"/>
       <c r="G4" s="1"/>
       <c r="H4" s="1"/>
-      <c r="I4" s="23"/>
-      <c r="J4" s="23"/>
+      <c r="I4" s="25"/>
+      <c r="J4" s="25"/>
     </row>
     <row r="5" ht="17.25" customHeight="1">
       <c r="A5" s="8">
@@ -3307,8 +3312,8 @@
       <c r="F5" s="1"/>
       <c r="G5" s="1"/>
       <c r="H5" s="1"/>
-      <c r="I5" s="23"/>
-      <c r="J5" s="23"/>
+      <c r="I5" s="25"/>
+      <c r="J5" s="25"/>
     </row>
     <row r="6" ht="17.25" customHeight="1">
       <c r="A6" s="8">
@@ -3323,8 +3328,8 @@
       <c r="F6" s="1"/>
       <c r="G6" s="1"/>
       <c r="H6" s="1"/>
-      <c r="I6" s="23"/>
-      <c r="J6" s="23"/>
+      <c r="I6" s="25"/>
+      <c r="J6" s="25"/>
     </row>
     <row r="7" ht="17.25" customHeight="1">
       <c r="A7" s="8">
@@ -3339,8 +3344,8 @@
       <c r="F7" s="1"/>
       <c r="G7" s="1"/>
       <c r="H7" s="1"/>
-      <c r="I7" s="23"/>
-      <c r="J7" s="23"/>
+      <c r="I7" s="25"/>
+      <c r="J7" s="25"/>
     </row>
     <row r="8" ht="17.25" customHeight="1">
       <c r="A8" s="8">
@@ -3355,8 +3360,8 @@
       <c r="F8" s="1"/>
       <c r="G8" s="1"/>
       <c r="H8" s="1"/>
-      <c r="I8" s="23"/>
-      <c r="J8" s="23"/>
+      <c r="I8" s="25"/>
+      <c r="J8" s="25"/>
     </row>
     <row r="9" ht="17.25" customHeight="1">
       <c r="A9" s="8">
@@ -3371,8 +3376,8 @@
       <c r="F9" s="1"/>
       <c r="G9" s="1"/>
       <c r="H9" s="1"/>
-      <c r="I9" s="23"/>
-      <c r="J9" s="23"/>
+      <c r="I9" s="25"/>
+      <c r="J9" s="25"/>
     </row>
     <row r="10" ht="17.25" customHeight="1">
       <c r="A10" s="8">
@@ -3387,14 +3392,14 @@
       <c r="F10" s="1"/>
       <c r="G10" s="1"/>
       <c r="H10" s="1"/>
-      <c r="I10" s="23"/>
-      <c r="J10" s="23"/>
+      <c r="I10" s="25"/>
+      <c r="J10" s="25"/>
     </row>
     <row r="11" ht="17.25" customHeight="1">
-      <c r="A11" s="10">
+      <c r="A11" s="22">
         <v>0.35199999999999998</v>
       </c>
-      <c r="B11" s="10">
+      <c r="B11" s="22">
         <v>0.112</v>
       </c>
       <c r="C11" s="1"/>
@@ -3403,8 +3408,8 @@
       <c r="F11" s="1"/>
       <c r="G11" s="1"/>
       <c r="H11" s="1"/>
-      <c r="I11" s="23"/>
-      <c r="J11" s="23"/>
+      <c r="I11" s="25"/>
+      <c r="J11" s="25"/>
     </row>
   </sheetData>
   <printOptions headings="0" gridLines="0"/>
@@ -3429,7 +3434,7 @@
   <cols>
     <col bestFit="1" customWidth="1" min="1" max="3" style="2" width="12.43357142857143"/>
     <col bestFit="1" customWidth="1" min="4" max="9" style="1" width="12.43357142857143"/>
-    <col bestFit="1" customWidth="1" min="10" max="11" style="12" width="12.43357142857143"/>
+    <col bestFit="1" customWidth="1" min="10" max="11" style="11" width="12.43357142857143"/>
   </cols>
   <sheetData>
     <row r="1" ht="17.25" customHeight="1">
@@ -3494,8 +3499,8 @@
       <c r="G3" s="1"/>
       <c r="H3" s="1"/>
       <c r="I3" s="1"/>
-      <c r="J3" s="23"/>
-      <c r="K3" s="23"/>
+      <c r="J3" s="25"/>
+      <c r="K3" s="25"/>
     </row>
     <row r="4" ht="17.25" customHeight="1">
       <c r="A4" s="8">
@@ -3513,8 +3518,8 @@
       <c r="G4" s="1"/>
       <c r="H4" s="1"/>
       <c r="I4" s="1"/>
-      <c r="J4" s="23"/>
-      <c r="K4" s="23"/>
+      <c r="J4" s="25"/>
+      <c r="K4" s="25"/>
     </row>
     <row r="5" ht="17.25" customHeight="1">
       <c r="A5" s="8">
@@ -3532,8 +3537,8 @@
       <c r="G5" s="1"/>
       <c r="H5" s="1"/>
       <c r="I5" s="1"/>
-      <c r="J5" s="23"/>
-      <c r="K5" s="23"/>
+      <c r="J5" s="25"/>
+      <c r="K5" s="25"/>
     </row>
     <row r="6" ht="17.25" customHeight="1">
       <c r="A6" s="8">
@@ -3551,8 +3556,8 @@
       <c r="G6" s="1"/>
       <c r="H6" s="1"/>
       <c r="I6" s="1"/>
-      <c r="J6" s="23"/>
-      <c r="K6" s="23"/>
+      <c r="J6" s="25"/>
+      <c r="K6" s="25"/>
     </row>
     <row r="7" ht="17.25" customHeight="1">
       <c r="A7" s="8"/>
@@ -3564,8 +3569,8 @@
       <c r="G7" s="1"/>
       <c r="H7" s="1"/>
       <c r="I7" s="1"/>
-      <c r="J7" s="23"/>
-      <c r="K7" s="23"/>
+      <c r="J7" s="25"/>
+      <c r="K7" s="25"/>
     </row>
     <row r="8" ht="17.25" customHeight="1">
       <c r="A8" s="8"/>
@@ -3577,8 +3582,8 @@
       <c r="G8" s="1"/>
       <c r="H8" s="1"/>
       <c r="I8" s="1"/>
-      <c r="J8" s="23"/>
-      <c r="K8" s="23"/>
+      <c r="J8" s="25"/>
+      <c r="K8" s="25"/>
     </row>
     <row r="9" ht="17.25" customHeight="1">
       <c r="A9" s="8"/>
@@ -3590,8 +3595,8 @@
       <c r="G9" s="1"/>
       <c r="H9" s="1"/>
       <c r="I9" s="1"/>
-      <c r="J9" s="23"/>
-      <c r="K9" s="23"/>
+      <c r="J9" s="25"/>
+      <c r="K9" s="25"/>
     </row>
     <row r="10" ht="17.25" customHeight="1">
       <c r="A10" s="8"/>
@@ -3603,8 +3608,8 @@
       <c r="G10" s="1"/>
       <c r="H10" s="1"/>
       <c r="I10" s="1"/>
-      <c r="J10" s="23"/>
-      <c r="K10" s="23"/>
+      <c r="J10" s="25"/>
+      <c r="K10" s="25"/>
     </row>
     <row r="11" ht="17.25" customHeight="1">
       <c r="A11" s="8"/>
@@ -3616,8 +3621,8 @@
       <c r="G11" s="1"/>
       <c r="H11" s="1"/>
       <c r="I11" s="1"/>
-      <c r="J11" s="23"/>
-      <c r="K11" s="23"/>
+      <c r="J11" s="25"/>
+      <c r="K11" s="25"/>
     </row>
   </sheetData>
   <printOptions headings="0" gridLines="0"/>

</xml_diff>

<commit_message>
creato grafico, rivedere con Marta
</commit_message>
<xml_diff>
--- a/URTI/urti_dati.xlsx
+++ b/URTI/urti_dati.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <workbookPr/>
   <bookViews>
-    <workbookView xWindow="360" yWindow="15" windowWidth="20955" windowHeight="9720" activeTab="3"/>
+    <workbookView xWindow="360" yWindow="15" windowWidth="20955" windowHeight="9720" activeTab="5"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" state="visible" r:id="rId1"/>
@@ -23,7 +23,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="50" uniqueCount="50">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="51" uniqueCount="51">
   <si>
     <t xml:space="preserve">massa carrello blu</t>
   </si>
@@ -112,12 +112,18 @@
     <t>m</t>
   </si>
   <si>
+    <t>viR</t>
+  </si>
+  <si>
     <t>vfR</t>
   </si>
   <si>
     <t>viB</t>
   </si>
   <si>
+    <t>vfB</t>
+  </si>
+  <si>
     <t>m_rosso</t>
   </si>
   <si>
@@ -149,9 +155,6 @@
   </si>
   <si>
     <t>deltaV/Vi</t>
-  </si>
-  <si>
-    <t>vfB</t>
   </si>
   <si>
     <t>F</t>
@@ -903,22 +906,22 @@
   <sheetData>
     <row r="1" ht="17.25" customHeight="1">
       <c r="A1" s="34" t="s">
-        <v>43</v>
+        <v>44</v>
       </c>
       <c r="B1" s="20" t="s">
-        <v>44</v>
+        <v>45</v>
       </c>
       <c r="C1" s="34" t="s">
-        <v>45</v>
+        <v>46</v>
       </c>
       <c r="D1" s="20" t="s">
-        <v>46</v>
+        <v>47</v>
       </c>
       <c r="E1" s="5" t="s">
-        <v>47</v>
+        <v>48</v>
       </c>
       <c r="F1" s="5" t="s">
-        <v>48</v>
+        <v>49</v>
       </c>
     </row>
     <row r="2" ht="17.25" customHeight="1">
@@ -926,14 +929,14 @@
         <v>1.1000000000000001</v>
       </c>
       <c r="B2" s="22">
-        <f t="shared" ref="B2:B7" si="26">A2/($E$2*9.81)</f>
+        <f t="shared" ref="B2:B7" si="20">A2/($E$2*9.81)</f>
         <v>0.22426095820591235</v>
       </c>
       <c r="C2" s="35">
         <v>1.3</v>
       </c>
       <c r="D2" s="22">
-        <f t="shared" ref="D2:D7" si="27">C2/($F$2*9.81)</f>
+        <f t="shared" ref="D2:D7" si="21">C2/($F$2*9.81)</f>
         <v>0.20231731135856074</v>
       </c>
       <c r="E2" s="8">
@@ -948,14 +951,14 @@
         <v>1.1000000000000001</v>
       </c>
       <c r="B3" s="22">
-        <f t="shared" si="26"/>
+        <f t="shared" si="20"/>
         <v>0.22426095820591235</v>
       </c>
       <c r="C3" s="35">
         <v>1.3999999999999999</v>
       </c>
       <c r="D3" s="22">
-        <f t="shared" si="27"/>
+        <f t="shared" si="21"/>
         <v>0.2178801814630654</v>
       </c>
       <c r="E3" s="25"/>
@@ -966,14 +969,14 @@
         <v>0.90000000000000002</v>
       </c>
       <c r="B4" s="22">
-        <f t="shared" si="26"/>
+        <f t="shared" si="20"/>
         <v>0.18348623853211007</v>
       </c>
       <c r="C4" s="35">
         <v>1.3999999999999999</v>
       </c>
       <c r="D4" s="22">
-        <f t="shared" si="27"/>
+        <f t="shared" si="21"/>
         <v>0.2178801814630654</v>
       </c>
       <c r="E4" s="25"/>
@@ -984,14 +987,14 @@
         <v>1.2</v>
       </c>
       <c r="B5" s="22">
-        <f t="shared" si="26"/>
+        <f t="shared" si="20"/>
         <v>0.24464831804281342</v>
       </c>
       <c r="C5" s="35">
         <v>1.5</v>
       </c>
       <c r="D5" s="22">
-        <f t="shared" si="27"/>
+        <f t="shared" si="21"/>
         <v>0.23344305156757009</v>
       </c>
       <c r="E5" s="25"/>
@@ -1002,14 +1005,14 @@
         <v>1.2</v>
       </c>
       <c r="B6" s="22">
-        <f t="shared" si="26"/>
+        <f t="shared" si="20"/>
         <v>0.24464831804281342</v>
       </c>
       <c r="C6" s="35">
         <v>1.3</v>
       </c>
       <c r="D6" s="22">
-        <f t="shared" si="27"/>
+        <f t="shared" si="21"/>
         <v>0.20231731135856074</v>
       </c>
       <c r="E6" s="25"/>
@@ -1020,14 +1023,14 @@
         <v>1</v>
       </c>
       <c r="B7" s="22">
-        <f t="shared" si="26"/>
+        <f t="shared" si="20"/>
         <v>0.2038735983690112</v>
       </c>
       <c r="C7" s="35">
         <v>1.3</v>
       </c>
       <c r="D7" s="22">
-        <f t="shared" si="27"/>
+        <f t="shared" si="21"/>
         <v>0.20231731135856074</v>
       </c>
       <c r="E7" s="25"/>
@@ -1077,7 +1080,7 @@
   <sheetData>
     <row r="1" ht="17.25" customHeight="1">
       <c r="A1" s="24" t="s">
-        <v>49</v>
+        <v>50</v>
       </c>
       <c r="B1" s="7" t="s">
         <v>28</v>
@@ -2401,12 +2404,14 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25"/>
   <cols>
-    <col bestFit="1" customWidth="1" min="1" max="4" style="11" width="12.43357142857143"/>
-    <col bestFit="1" customWidth="1" min="5" max="10" style="1" width="12.43357142857143"/>
+    <col bestFit="1" customWidth="1" min="2" max="3" style="11" width="12.43357142857143"/>
+    <col customWidth="1" min="4" max="4" style="11" width="12.43357142857143"/>
+    <col bestFit="1" customWidth="1" min="5" max="6" style="11" width="12.43357142857143"/>
+    <col bestFit="1" customWidth="1" min="7" max="12" style="1" width="12.43357142857143"/>
   </cols>
   <sheetData>
     <row r="1" ht="17.25" customHeight="1">
-      <c r="A1" s="5" t="s">
+      <c r="A1" t="s">
         <v>29</v>
       </c>
       <c r="B1" s="5" t="s">
@@ -2418,324 +2423,345 @@
       <c r="D1" s="5" t="s">
         <v>32</v>
       </c>
-      <c r="E1" s="20" t="s">
+      <c r="E1" s="5" t="s">
+        <v>33</v>
+      </c>
+      <c r="F1" s="5" t="s">
+        <v>34</v>
+      </c>
+      <c r="G1" s="20" t="s">
         <v>25</v>
       </c>
-      <c r="F1" s="20" t="s">
+      <c r="H1" s="20" t="s">
         <v>26</v>
       </c>
-      <c r="G1" s="20" t="s">
+      <c r="I1" s="20" t="s">
         <v>27</v>
       </c>
-      <c r="H1" s="20" t="s">
-        <v>33</v>
-      </c>
-      <c r="I1" s="20" t="s">
-        <v>34</v>
-      </c>
       <c r="J1" s="20" t="s">
+        <v>35</v>
+      </c>
+      <c r="K1" s="20" t="s">
+        <v>36</v>
+      </c>
+      <c r="L1" s="20" t="s">
         <v>23</v>
       </c>
     </row>
     <row r="2" ht="17.25" customHeight="1">
-      <c r="A2" s="8">
+      <c r="A2" s="17">
+        <v>0</v>
+      </c>
+      <c r="B2" s="8">
         <v>0.44900000000000001</v>
       </c>
-      <c r="B2" s="8">
+      <c r="C2" s="8">
         <v>0.46600000000000003</v>
       </c>
-      <c r="C2" s="8">
+      <c r="D2" s="8">
+        <v>0</v>
+      </c>
+      <c r="E2" s="8">
         <v>0.27300000000000002</v>
       </c>
-      <c r="D2" s="8">
+      <c r="F2" s="8">
         <v>0.27000000000000002</v>
       </c>
-      <c r="E2" s="23">
-        <f t="shared" ref="E2:E9" si="12">0.5*($D$2)*B2*B2</f>
+      <c r="G2" s="23">
+        <f>0.5*($F$2)*C2*C2</f>
         <v>0.029316060000000005</v>
       </c>
-      <c r="F2" s="23">
-        <f t="shared" ref="F2:F9" si="13">0.5*$C$2*A2*A2</f>
+      <c r="H2" s="23">
+        <f>0.5*$E$2*B2*B2</f>
         <v>0.027518536500000003</v>
       </c>
-      <c r="G2" s="8">
-        <f t="shared" ref="G2:G9" si="14">F2-E2</f>
+      <c r="I2" s="8">
+        <f>H2-G2</f>
         <v>-0.001797523500000002</v>
       </c>
-      <c r="H2" s="23">
-        <f t="shared" ref="H2:H9" si="15">$D$2*B2</f>
+      <c r="J2" s="23">
+        <f>$F$2*C2</f>
         <v>0.12582000000000002</v>
       </c>
-      <c r="I2" s="23">
-        <f t="shared" ref="I2:I9" si="16">$C$2*A2</f>
+      <c r="K2" s="23">
+        <f>$E$2*B2</f>
         <v>0.12257700000000001</v>
       </c>
-      <c r="J2" s="8">
-        <f t="shared" ref="J2:J9" si="17">I2-H2</f>
+      <c r="L2" s="8">
+        <f>K2-J2</f>
         <v>-0.0032430000000000098</v>
       </c>
     </row>
     <row r="3" ht="17.25" customHeight="1">
-      <c r="A3" s="8">
+      <c r="B3" s="8">
         <v>0.63</v>
       </c>
-      <c r="B3" s="8">
+      <c r="C3" s="8">
         <v>0.65800000000000003</v>
       </c>
-      <c r="C3" s="25"/>
-      <c r="D3" s="25"/>
-      <c r="E3" s="23">
-        <f t="shared" si="12"/>
+      <c r="D3" s="8"/>
+      <c r="E3" s="25"/>
+      <c r="F3" s="25"/>
+      <c r="G3" s="23">
+        <f>0.5*($F$2)*C3*C3</f>
         <v>0.058450140000000005</v>
       </c>
-      <c r="F3" s="23">
-        <f t="shared" si="13"/>
+      <c r="H3" s="23">
+        <f>0.5*$E$2*B3*B3</f>
         <v>0.054176849999999999</v>
       </c>
-      <c r="G3" s="8">
-        <f t="shared" si="14"/>
+      <c r="I3" s="8">
+        <f>H3-G3</f>
         <v>-0.004273290000000006</v>
       </c>
-      <c r="H3" s="23">
-        <f t="shared" si="15"/>
+      <c r="J3" s="23">
+        <f>$F$2*C3</f>
         <v>0.17766000000000001</v>
       </c>
-      <c r="I3" s="23">
-        <f t="shared" si="16"/>
+      <c r="K3" s="23">
+        <f>$E$2*B3</f>
         <v>0.17199</v>
       </c>
-      <c r="J3" s="8">
-        <f t="shared" si="17"/>
+      <c r="L3" s="8">
+        <f>K3-J3</f>
         <v>-0.0056700000000000084</v>
       </c>
     </row>
     <row r="4" ht="17.25" customHeight="1">
-      <c r="A4" s="8">
+      <c r="B4" s="8">
         <v>0.624</v>
       </c>
-      <c r="B4" s="8">
+      <c r="C4" s="8">
         <v>0.64800000000000002</v>
       </c>
-      <c r="C4" s="25"/>
-      <c r="D4" s="25"/>
-      <c r="E4" s="23">
-        <f t="shared" si="12"/>
+      <c r="D4" s="8"/>
+      <c r="E4" s="25"/>
+      <c r="F4" s="25"/>
+      <c r="G4" s="23">
+        <f>0.5*($F$2)*C4*C4</f>
         <v>0.056687040000000001</v>
       </c>
-      <c r="F4" s="23">
-        <f t="shared" si="13"/>
+      <c r="H4" s="23">
+        <f>0.5*$E$2*B4*B4</f>
         <v>0.053149823999999998</v>
       </c>
-      <c r="G4" s="8">
-        <f t="shared" si="14"/>
+      <c r="I4" s="8">
+        <f>H4-G4</f>
         <v>-0.0035372160000000027</v>
       </c>
-      <c r="H4" s="23">
-        <f t="shared" si="15"/>
+      <c r="J4" s="23">
+        <f>$F$2*C4</f>
         <v>0.17496</v>
       </c>
-      <c r="I4" s="23">
-        <f t="shared" si="16"/>
+      <c r="K4" s="23">
+        <f>$E$2*B4</f>
         <v>0.170352</v>
       </c>
-      <c r="J4" s="8">
-        <f t="shared" si="17"/>
+      <c r="L4" s="8">
+        <f>K4-J4</f>
         <v>-0.004608000000000001</v>
       </c>
     </row>
     <row r="5" ht="17.25" customHeight="1">
-      <c r="A5" s="8">
+      <c r="B5" s="8">
         <v>0.56999999999999995</v>
       </c>
-      <c r="B5" s="8">
+      <c r="C5" s="8">
         <v>0.59399999999999997</v>
       </c>
-      <c r="C5" s="25"/>
-      <c r="D5" s="25"/>
-      <c r="E5" s="23">
-        <f t="shared" si="12"/>
+      <c r="D5" s="8"/>
+      <c r="E5" s="25"/>
+      <c r="F5" s="25"/>
+      <c r="G5" s="23">
+        <f>0.5*($F$2)*C5*C5</f>
         <v>0.047632859999999999</v>
       </c>
-      <c r="F5" s="23">
-        <f t="shared" si="13"/>
+      <c r="H5" s="23">
+        <f>0.5*$E$2*B5*B5</f>
         <v>0.044348849999999995</v>
       </c>
-      <c r="G5" s="8">
-        <f t="shared" si="14"/>
+      <c r="I5" s="8">
+        <f>H5-G5</f>
         <v>-0.0032840100000000039</v>
       </c>
-      <c r="H5" s="23">
-        <f t="shared" si="15"/>
+      <c r="J5" s="23">
+        <f>$F$2*C5</f>
         <v>0.16037999999999999</v>
       </c>
-      <c r="I5" s="23">
-        <f t="shared" si="16"/>
+      <c r="K5" s="23">
+        <f>$E$2*B5</f>
         <v>0.15561</v>
       </c>
-      <c r="J5" s="8">
-        <f t="shared" si="17"/>
+      <c r="L5" s="8">
+        <f>K5-J5</f>
         <v>-0.0047699999999999965</v>
       </c>
     </row>
     <row r="6" ht="17.25" customHeight="1">
-      <c r="A6" s="8">
+      <c r="B6" s="8">
         <v>0.58799999999999997</v>
       </c>
-      <c r="B6" s="8">
+      <c r="C6" s="8">
         <v>0.60899999999999999</v>
       </c>
-      <c r="C6" s="25"/>
-      <c r="D6" s="25"/>
-      <c r="E6" s="23">
-        <f t="shared" si="12"/>
+      <c r="D6" s="8"/>
+      <c r="E6" s="25"/>
+      <c r="F6" s="25"/>
+      <c r="G6" s="23">
+        <f>0.5*($F$2)*C6*C6</f>
         <v>0.050068935000000002</v>
       </c>
-      <c r="F6" s="23">
-        <f t="shared" si="13"/>
+      <c r="H6" s="23">
+        <f>0.5*$E$2*B6*B6</f>
         <v>0.047194055999999998</v>
       </c>
-      <c r="G6" s="8">
-        <f t="shared" si="14"/>
+      <c r="I6" s="8">
+        <f>H6-G6</f>
         <v>-0.0028748790000000038</v>
       </c>
-      <c r="H6" s="23">
-        <f t="shared" si="15"/>
+      <c r="J6" s="23">
+        <f>$F$2*C6</f>
         <v>0.16443000000000002</v>
       </c>
-      <c r="I6" s="23">
-        <f t="shared" si="16"/>
+      <c r="K6" s="23">
+        <f>$E$2*B6</f>
         <v>0.160524</v>
       </c>
-      <c r="J6" s="8">
-        <f t="shared" si="17"/>
+      <c r="L6" s="8">
+        <f>K6-J6</f>
         <v>-0.0039060000000000206</v>
       </c>
     </row>
     <row r="7" ht="17.25" customHeight="1">
-      <c r="A7" s="8">
+      <c r="B7" s="8">
         <v>0.80900000000000005</v>
       </c>
-      <c r="B7" s="8">
+      <c r="C7" s="8">
         <v>0.83699999999999997</v>
       </c>
-      <c r="C7" s="25"/>
-      <c r="D7" s="25"/>
-      <c r="E7" s="23">
-        <f t="shared" si="12"/>
+      <c r="D7" s="8"/>
+      <c r="E7" s="25"/>
+      <c r="F7" s="25"/>
+      <c r="G7" s="23">
+        <f>0.5*($F$2)*C7*C7</f>
         <v>0.094576814999999995</v>
       </c>
-      <c r="F7" s="23">
-        <f t="shared" si="13"/>
+      <c r="H7" s="23">
+        <f>0.5*$E$2*B7*B7</f>
         <v>0.089336656500000014</v>
       </c>
-      <c r="G7" s="8">
-        <f t="shared" si="14"/>
+      <c r="I7" s="8">
+        <f>H7-G7</f>
         <v>-0.0052401584999999806</v>
       </c>
-      <c r="H7" s="23">
-        <f t="shared" si="15"/>
+      <c r="J7" s="23">
+        <f>$F$2*C7</f>
         <v>0.22599</v>
       </c>
-      <c r="I7" s="23">
-        <f t="shared" si="16"/>
+      <c r="K7" s="23">
+        <f>$E$2*B7</f>
         <v>0.22085700000000003</v>
       </c>
-      <c r="J7" s="8">
-        <f t="shared" si="17"/>
+      <c r="L7" s="8">
+        <f>K7-J7</f>
         <v>-0.0051329999999999709</v>
       </c>
     </row>
     <row r="8" ht="17.25" customHeight="1">
-      <c r="A8" s="8">
+      <c r="B8" s="8">
         <v>0.86299999999999999</v>
       </c>
-      <c r="B8" s="8">
+      <c r="C8" s="8">
         <v>0.878</v>
       </c>
-      <c r="C8" s="25"/>
-      <c r="D8" s="25"/>
-      <c r="E8" s="23">
-        <f t="shared" si="12"/>
+      <c r="D8" s="8"/>
+      <c r="E8" s="25"/>
+      <c r="F8" s="25"/>
+      <c r="G8" s="23">
+        <f>0.5*($F$2)*C8*C8</f>
         <v>0.10406934000000001</v>
       </c>
-      <c r="F8" s="23">
-        <f t="shared" si="13"/>
+      <c r="H8" s="23">
+        <f>0.5*$E$2*B8*B8</f>
         <v>0.1016609685</v>
       </c>
-      <c r="G8" s="8">
-        <f t="shared" si="14"/>
+      <c r="I8" s="8">
+        <f>H8-G8</f>
         <v>-0.0024083715000000061</v>
       </c>
-      <c r="H8" s="23">
-        <f t="shared" si="15"/>
+      <c r="J8" s="23">
+        <f>$F$2*C8</f>
         <v>0.23706000000000002</v>
       </c>
-      <c r="I8" s="23">
-        <f t="shared" si="16"/>
+      <c r="K8" s="23">
+        <f>$E$2*B8</f>
         <v>0.235599</v>
       </c>
-      <c r="J8" s="8">
-        <f t="shared" si="17"/>
+      <c r="L8" s="8">
+        <f>K8-J8</f>
         <v>-0.0014610000000000178</v>
       </c>
     </row>
     <row r="9" ht="17.25" customHeight="1">
-      <c r="A9" s="8">
+      <c r="B9" s="8">
         <v>0.66300000000000003</v>
       </c>
-      <c r="B9" s="8">
+      <c r="C9" s="8">
         <v>0.69099999999999995</v>
       </c>
-      <c r="C9" s="25"/>
-      <c r="D9" s="25"/>
-      <c r="E9" s="23">
-        <f t="shared" si="12"/>
+      <c r="D9" s="8"/>
+      <c r="E9" s="25"/>
+      <c r="F9" s="25"/>
+      <c r="G9" s="23">
+        <f>0.5*($F$2)*C9*C9</f>
         <v>0.064459934999999996</v>
       </c>
-      <c r="F9" s="23">
-        <f t="shared" si="13"/>
+      <c r="H9" s="23">
+        <f>0.5*$E$2*B9*B9</f>
         <v>0.060001168500000007</v>
       </c>
-      <c r="G9" s="8">
-        <f t="shared" si="14"/>
+      <c r="I9" s="8">
+        <f>H9-G9</f>
         <v>-0.0044587664999999888</v>
       </c>
-      <c r="H9" s="23">
-        <f t="shared" si="15"/>
+      <c r="J9" s="23">
+        <f>$F$2*C9</f>
         <v>0.18656999999999999</v>
       </c>
-      <c r="I9" s="23">
-        <f t="shared" si="16"/>
+      <c r="K9" s="23">
+        <f>$E$2*B9</f>
         <v>0.18099900000000002</v>
       </c>
-      <c r="J9" s="8">
-        <f t="shared" si="17"/>
+      <c r="L9" s="8">
+        <f>K9-J9</f>
         <v>-0.0055709999999999649</v>
       </c>
     </row>
     <row r="10" ht="17.25" customHeight="1">
-      <c r="A10" s="8"/>
       <c r="B10" s="8"/>
-      <c r="C10" s="25"/>
-      <c r="D10" s="25"/>
-      <c r="E10" s="26"/>
-      <c r="F10" s="26"/>
-      <c r="G10" s="25"/>
+      <c r="C10" s="8"/>
+      <c r="D10" s="8"/>
+      <c r="E10" s="25"/>
+      <c r="F10" s="25"/>
+      <c r="G10" s="26"/>
       <c r="H10" s="26"/>
-      <c r="I10" s="26"/>
-      <c r="J10" s="25"/>
+      <c r="I10" s="25"/>
+      <c r="J10" s="26"/>
+      <c r="K10" s="26"/>
+      <c r="L10" s="25"/>
     </row>
     <row r="11" ht="17.25" customHeight="1">
-      <c r="A11" s="25"/>
       <c r="B11" s="25"/>
       <c r="C11" s="25"/>
       <c r="D11" s="25"/>
-      <c r="E11" s="26"/>
-      <c r="F11" s="26"/>
-      <c r="G11" s="25"/>
+      <c r="E11" s="25"/>
+      <c r="F11" s="25"/>
+      <c r="G11" s="26"/>
       <c r="H11" s="26"/>
-      <c r="I11" s="26"/>
-      <c r="J11" s="25"/>
+      <c r="I11" s="25"/>
+      <c r="J11" s="26"/>
+      <c r="K11" s="26"/>
+      <c r="L11" s="25"/>
     </row>
   </sheetData>
   <printOptions headings="0" gridLines="0"/>
@@ -2766,19 +2792,19 @@
   <sheetData>
     <row r="1" ht="17.25" customHeight="1">
       <c r="A1" s="25" t="s">
-        <v>35</v>
+        <v>37</v>
       </c>
       <c r="B1" s="25" t="s">
-        <v>36</v>
+        <v>38</v>
       </c>
       <c r="C1" s="5" t="s">
-        <v>37</v>
+        <v>39</v>
       </c>
       <c r="D1" s="5" t="s">
-        <v>38</v>
+        <v>40</v>
       </c>
       <c r="E1" s="29" t="s">
-        <v>39</v>
+        <v>41</v>
       </c>
       <c r="F1" s="28" t="s">
         <v>25</v>
@@ -2790,16 +2816,16 @@
         <v>27</v>
       </c>
       <c r="I1" s="28" t="s">
-        <v>40</v>
+        <v>42</v>
       </c>
       <c r="J1" s="28" t="s">
-        <v>41</v>
+        <v>43</v>
       </c>
       <c r="K1" s="28" t="s">
-        <v>33</v>
+        <v>35</v>
       </c>
       <c r="L1" s="28" t="s">
-        <v>34</v>
+        <v>36</v>
       </c>
       <c r="M1" s="28" t="s">
         <v>23</v>
@@ -2822,35 +2848,35 @@
         <v>0</v>
       </c>
       <c r="F2" s="23">
-        <f t="shared" ref="F2:F9" si="18">0.5*$D$2*A2*A2</f>
+        <f t="shared" ref="F2:F9" si="12">0.5*$D$2*A2*A2</f>
         <v>0.016907149999999999</v>
       </c>
       <c r="G2" s="23">
-        <f t="shared" ref="G2:G9" si="19">0.5*($C$2+$D$2)*B2*B2</f>
+        <f t="shared" ref="G2:G9" si="13">0.5*($C$2+$D$2)*B2*B2</f>
         <v>0.0078734739999999984</v>
       </c>
       <c r="H2" s="8">
-        <f t="shared" ref="H2:H9" si="20">G2-F2</f>
+        <f t="shared" ref="H2:H9" si="14">G2-F2</f>
         <v>-0.0090336760000000009</v>
       </c>
       <c r="I2" s="8">
-        <f t="shared" ref="I2:I9" si="21">B2-A2</f>
+        <f t="shared" ref="I2:I9" si="15">B2-A2</f>
         <v>0.192</v>
       </c>
       <c r="J2" s="31">
-        <f t="shared" ref="J2:J9" si="22">I2/A2</f>
+        <f t="shared" ref="J2:J9" si="16">I2/A2</f>
         <v>-0.51891891891891895</v>
       </c>
       <c r="K2" s="8">
-        <f t="shared" ref="K2:K9" si="23">$D$2*A2</f>
+        <f t="shared" ref="K2:K9" si="17">$D$2*A2</f>
         <v>-0.091389999999999999</v>
       </c>
       <c r="L2" s="8">
-        <f t="shared" ref="L2:L9" si="24">($C$2+$D$2)*B2</f>
+        <f t="shared" ref="L2:L9" si="18">($C$2+$D$2)*B2</f>
         <v>-0.088465999999999989</v>
       </c>
       <c r="M2" s="8">
-        <f t="shared" ref="M2:M9" si="25">L2-K2</f>
+        <f t="shared" ref="M2:M9" si="19">L2-K2</f>
         <v>0.0029240000000000099</v>
       </c>
     </row>
@@ -2865,35 +2891,35 @@
       <c r="D3" s="25"/>
       <c r="E3" s="32"/>
       <c r="F3" s="23">
+        <f t="shared" si="12"/>
+        <v>0.031122493999999997</v>
+      </c>
+      <c r="G3" s="23">
+        <f t="shared" si="13"/>
+        <v>0.014673676499999998</v>
+      </c>
+      <c r="H3" s="8">
+        <f t="shared" si="14"/>
+        <v>-0.016448817499999997</v>
+      </c>
+      <c r="I3" s="8">
+        <f t="shared" si="15"/>
+        <v>0.25900000000000001</v>
+      </c>
+      <c r="J3" s="31">
+        <f t="shared" si="16"/>
+        <v>-0.51593625498007967</v>
+      </c>
+      <c r="K3" s="8">
+        <f t="shared" si="17"/>
+        <v>-0.12399399999999999</v>
+      </c>
+      <c r="L3" s="8">
         <f t="shared" si="18"/>
-        <v>0.031122493999999997</v>
-      </c>
-      <c r="G3" s="23">
+        <v>-0.12077099999999999</v>
+      </c>
+      <c r="M3" s="8">
         <f t="shared" si="19"/>
-        <v>0.014673676499999998</v>
-      </c>
-      <c r="H3" s="8">
-        <f t="shared" si="20"/>
-        <v>-0.016448817499999997</v>
-      </c>
-      <c r="I3" s="8">
-        <f t="shared" si="21"/>
-        <v>0.25900000000000001</v>
-      </c>
-      <c r="J3" s="31">
-        <f t="shared" si="22"/>
-        <v>-0.51593625498007967</v>
-      </c>
-      <c r="K3" s="8">
-        <f t="shared" si="23"/>
-        <v>-0.12399399999999999</v>
-      </c>
-      <c r="L3" s="8">
-        <f t="shared" si="24"/>
-        <v>-0.12077099999999999</v>
-      </c>
-      <c r="M3" s="8">
-        <f t="shared" si="25"/>
         <v>0.0032230000000000036</v>
       </c>
     </row>
@@ -2908,35 +2934,35 @@
       <c r="D4" s="25"/>
       <c r="E4" s="32"/>
       <c r="F4" s="23">
+        <f t="shared" si="12"/>
+        <v>0.046710787499999996</v>
+      </c>
+      <c r="G4" s="23">
+        <f t="shared" si="13"/>
+        <v>0.022664193999999999</v>
+      </c>
+      <c r="H4" s="8">
+        <f t="shared" si="14"/>
+        <v>-0.024046593499999998</v>
+      </c>
+      <c r="I4" s="8">
+        <f t="shared" si="15"/>
+        <v>0.313</v>
+      </c>
+      <c r="J4" s="31">
+        <f t="shared" si="16"/>
+        <v>-0.50894308943089428</v>
+      </c>
+      <c r="K4" s="8">
+        <f t="shared" si="17"/>
+        <v>-0.15190499999999998</v>
+      </c>
+      <c r="L4" s="8">
         <f t="shared" si="18"/>
-        <v>0.046710787499999996</v>
-      </c>
-      <c r="G4" s="23">
+        <v>-0.15009400000000001</v>
+      </c>
+      <c r="M4" s="8">
         <f t="shared" si="19"/>
-        <v>0.022664193999999999</v>
-      </c>
-      <c r="H4" s="8">
-        <f t="shared" si="20"/>
-        <v>-0.024046593499999998</v>
-      </c>
-      <c r="I4" s="8">
-        <f t="shared" si="21"/>
-        <v>0.313</v>
-      </c>
-      <c r="J4" s="31">
-        <f t="shared" si="22"/>
-        <v>-0.50894308943089428</v>
-      </c>
-      <c r="K4" s="8">
-        <f t="shared" si="23"/>
-        <v>-0.15190499999999998</v>
-      </c>
-      <c r="L4" s="8">
-        <f t="shared" si="24"/>
-        <v>-0.15009400000000001</v>
-      </c>
-      <c r="M4" s="8">
-        <f t="shared" si="25"/>
         <v>0.0018109999999999793</v>
       </c>
     </row>
@@ -2951,35 +2977,35 @@
       <c r="D5" s="25"/>
       <c r="E5" s="32"/>
       <c r="F5" s="23">
+        <f t="shared" si="12"/>
+        <v>0.053146496000000008</v>
+      </c>
+      <c r="G5" s="23">
+        <f t="shared" si="13"/>
+        <v>0.025446400000000004</v>
+      </c>
+      <c r="H5" s="8">
+        <f t="shared" si="14"/>
+        <v>-0.027700096000000004</v>
+      </c>
+      <c r="I5" s="8">
+        <f t="shared" si="15"/>
+        <v>0.33600000000000002</v>
+      </c>
+      <c r="J5" s="31">
+        <f t="shared" si="16"/>
+        <v>-0.51219512195121952</v>
+      </c>
+      <c r="K5" s="8">
+        <f t="shared" si="17"/>
+        <v>-0.16203200000000001</v>
+      </c>
+      <c r="L5" s="8">
         <f t="shared" si="18"/>
-        <v>0.053146496000000008</v>
-      </c>
-      <c r="G5" s="23">
+        <v>-0.15904000000000001</v>
+      </c>
+      <c r="M5" s="8">
         <f t="shared" si="19"/>
-        <v>0.025446400000000004</v>
-      </c>
-      <c r="H5" s="8">
-        <f t="shared" si="20"/>
-        <v>-0.027700096000000004</v>
-      </c>
-      <c r="I5" s="8">
-        <f t="shared" si="21"/>
-        <v>0.33600000000000002</v>
-      </c>
-      <c r="J5" s="31">
-        <f t="shared" si="22"/>
-        <v>-0.51219512195121952</v>
-      </c>
-      <c r="K5" s="8">
-        <f t="shared" si="23"/>
-        <v>-0.16203200000000001</v>
-      </c>
-      <c r="L5" s="8">
-        <f t="shared" si="24"/>
-        <v>-0.15904000000000001</v>
-      </c>
-      <c r="M5" s="8">
-        <f t="shared" si="25"/>
         <v>0.0029919999999999947</v>
       </c>
     </row>
@@ -2994,35 +3020,35 @@
       <c r="D6" s="25"/>
       <c r="E6" s="32"/>
       <c r="F6" s="23">
+        <f t="shared" si="12"/>
+        <v>0.036952311500000001</v>
+      </c>
+      <c r="G6" s="23">
+        <f t="shared" si="13"/>
+        <v>0.017319456000000004</v>
+      </c>
+      <c r="H6" s="8">
+        <f t="shared" si="14"/>
+        <v>-0.019632855499999997</v>
+      </c>
+      <c r="I6" s="8">
+        <f t="shared" si="15"/>
+        <v>0.28300000000000003</v>
+      </c>
+      <c r="J6" s="31">
+        <f t="shared" si="16"/>
+        <v>-0.51736745886654478</v>
+      </c>
+      <c r="K6" s="8">
+        <f t="shared" si="17"/>
+        <v>-0.13510900000000001</v>
+      </c>
+      <c r="L6" s="8">
         <f t="shared" si="18"/>
-        <v>0.036952311500000001</v>
-      </c>
-      <c r="G6" s="23">
+        <v>-0.13120800000000002</v>
+      </c>
+      <c r="M6" s="8">
         <f t="shared" si="19"/>
-        <v>0.017319456000000004</v>
-      </c>
-      <c r="H6" s="8">
-        <f t="shared" si="20"/>
-        <v>-0.019632855499999997</v>
-      </c>
-      <c r="I6" s="8">
-        <f t="shared" si="21"/>
-        <v>0.28300000000000003</v>
-      </c>
-      <c r="J6" s="31">
-        <f t="shared" si="22"/>
-        <v>-0.51736745886654478</v>
-      </c>
-      <c r="K6" s="8">
-        <f t="shared" si="23"/>
-        <v>-0.13510900000000001</v>
-      </c>
-      <c r="L6" s="8">
-        <f t="shared" si="24"/>
-        <v>-0.13120800000000002</v>
-      </c>
-      <c r="M6" s="8">
-        <f t="shared" si="25"/>
         <v>0.0039009999999999878</v>
       </c>
     </row>
@@ -3037,35 +3063,35 @@
       <c r="D7" s="25"/>
       <c r="E7" s="32"/>
       <c r="F7" s="23">
+        <f t="shared" si="12"/>
+        <v>0.056938563500000004</v>
+      </c>
+      <c r="G7" s="23">
+        <f t="shared" si="13"/>
+        <v>0.027061650000000003</v>
+      </c>
+      <c r="H7" s="8">
+        <f t="shared" si="14"/>
+        <v>-0.029876913500000001</v>
+      </c>
+      <c r="I7" s="8">
+        <f t="shared" si="15"/>
+        <v>0.34900000000000003</v>
+      </c>
+      <c r="J7" s="31">
+        <f t="shared" si="16"/>
+        <v>-0.51399116347569962</v>
+      </c>
+      <c r="K7" s="8">
+        <f t="shared" si="17"/>
+        <v>-0.167713</v>
+      </c>
+      <c r="L7" s="8">
         <f t="shared" si="18"/>
-        <v>0.056938563500000004</v>
-      </c>
-      <c r="G7" s="23">
+        <v>-0.16401000000000002</v>
+      </c>
+      <c r="M7" s="8">
         <f t="shared" si="19"/>
-        <v>0.027061650000000003</v>
-      </c>
-      <c r="H7" s="8">
-        <f t="shared" si="20"/>
-        <v>-0.029876913500000001</v>
-      </c>
-      <c r="I7" s="8">
-        <f t="shared" si="21"/>
-        <v>0.34900000000000003</v>
-      </c>
-      <c r="J7" s="31">
-        <f t="shared" si="22"/>
-        <v>-0.51399116347569962</v>
-      </c>
-      <c r="K7" s="8">
-        <f t="shared" si="23"/>
-        <v>-0.167713</v>
-      </c>
-      <c r="L7" s="8">
-        <f t="shared" si="24"/>
-        <v>-0.16401000000000002</v>
-      </c>
-      <c r="M7" s="8">
-        <f t="shared" si="25"/>
         <v>0.0037029999999999841</v>
       </c>
     </row>
@@ -3080,35 +3106,35 @@
       <c r="D8" s="25"/>
       <c r="E8" s="32"/>
       <c r="F8" s="23">
+        <f t="shared" si="12"/>
+        <v>0.038178296000000007</v>
+      </c>
+      <c r="G8" s="23">
+        <f t="shared" si="13"/>
+        <v>0.017981708500000002</v>
+      </c>
+      <c r="H8" s="8">
+        <f t="shared" si="14"/>
+        <v>-0.020196587500000005</v>
+      </c>
+      <c r="I8" s="8">
+        <f t="shared" si="15"/>
+        <v>0.28700000000000003</v>
+      </c>
+      <c r="J8" s="31">
+        <f t="shared" si="16"/>
+        <v>-0.51618705035971224</v>
+      </c>
+      <c r="K8" s="8">
+        <f t="shared" si="17"/>
+        <v>-0.13733200000000001</v>
+      </c>
+      <c r="L8" s="8">
         <f t="shared" si="18"/>
-        <v>0.038178296000000007</v>
-      </c>
-      <c r="G8" s="23">
+        <v>-0.13369300000000001</v>
+      </c>
+      <c r="M8" s="8">
         <f t="shared" si="19"/>
-        <v>0.017981708500000002</v>
-      </c>
-      <c r="H8" s="8">
-        <f t="shared" si="20"/>
-        <v>-0.020196587500000005</v>
-      </c>
-      <c r="I8" s="8">
-        <f t="shared" si="21"/>
-        <v>0.28700000000000003</v>
-      </c>
-      <c r="J8" s="31">
-        <f t="shared" si="22"/>
-        <v>-0.51618705035971224</v>
-      </c>
-      <c r="K8" s="8">
-        <f t="shared" si="23"/>
-        <v>-0.13733200000000001</v>
-      </c>
-      <c r="L8" s="8">
-        <f t="shared" si="24"/>
-        <v>-0.13369300000000001</v>
-      </c>
-      <c r="M8" s="8">
-        <f t="shared" si="25"/>
         <v>0.0036390000000000033</v>
       </c>
     </row>
@@ -3123,35 +3149,35 @@
       <c r="D9" s="25"/>
       <c r="E9" s="32"/>
       <c r="F9" s="23">
+        <f t="shared" si="12"/>
+        <v>0.035348787500000006</v>
+      </c>
+      <c r="G9" s="23">
+        <f t="shared" si="13"/>
+        <v>0.0167986</v>
+      </c>
+      <c r="H9" s="8">
+        <f t="shared" si="14"/>
+        <v>-0.018550187500000006</v>
+      </c>
+      <c r="I9" s="8">
+        <f t="shared" si="15"/>
+        <v>0.27500000000000002</v>
+      </c>
+      <c r="J9" s="31">
+        <f t="shared" si="16"/>
+        <v>-0.5140186915887851</v>
+      </c>
+      <c r="K9" s="8">
+        <f t="shared" si="17"/>
+        <v>-0.13214500000000001</v>
+      </c>
+      <c r="L9" s="8">
         <f t="shared" si="18"/>
-        <v>0.035348787500000006</v>
-      </c>
-      <c r="G9" s="23">
+        <v>-0.12922</v>
+      </c>
+      <c r="M9" s="8">
         <f t="shared" si="19"/>
-        <v>0.0167986</v>
-      </c>
-      <c r="H9" s="8">
-        <f t="shared" si="20"/>
-        <v>-0.018550187500000006</v>
-      </c>
-      <c r="I9" s="8">
-        <f t="shared" si="21"/>
-        <v>0.27500000000000002</v>
-      </c>
-      <c r="J9" s="31">
-        <f t="shared" si="22"/>
-        <v>-0.5140186915887851</v>
-      </c>
-      <c r="K9" s="8">
-        <f t="shared" si="23"/>
-        <v>-0.13214500000000001</v>
-      </c>
-      <c r="L9" s="8">
-        <f t="shared" si="24"/>
-        <v>-0.12922</v>
-      </c>
-      <c r="M9" s="8">
-        <f t="shared" si="25"/>
         <v>0.0029250000000000109</v>
       </c>
     </row>
@@ -3226,7 +3252,7 @@
   <sheetData>
     <row r="1" ht="17.25" customHeight="1">
       <c r="A1" s="24" t="s">
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="B1" s="24" t="s">
         <v>22</v>
@@ -3238,10 +3264,10 @@
       <c r="G1" s="1"/>
       <c r="H1" s="1"/>
       <c r="I1" s="5" t="s">
-        <v>37</v>
+        <v>39</v>
       </c>
       <c r="J1" s="5" t="s">
-        <v>38</v>
+        <v>40</v>
       </c>
     </row>
     <row r="2" ht="17.25" customHeight="1">
@@ -3436,13 +3462,13 @@
   <sheetData>
     <row r="1" ht="17.25" customHeight="1">
       <c r="A1" s="5" t="s">
+        <v>31</v>
+      </c>
+      <c r="B1" s="5" t="s">
+        <v>32</v>
+      </c>
+      <c r="C1" s="5" t="s">
         <v>30</v>
-      </c>
-      <c r="B1" s="5" t="s">
-        <v>42</v>
-      </c>
-      <c r="C1" s="5" t="s">
-        <v>29</v>
       </c>
       <c r="D1" s="1"/>
       <c r="E1" s="1"/>
@@ -3451,10 +3477,10 @@
       <c r="H1" s="1"/>
       <c r="I1" s="1"/>
       <c r="J1" s="5" t="s">
-        <v>37</v>
+        <v>39</v>
       </c>
       <c r="K1" s="5" t="s">
-        <v>38</v>
+        <v>40</v>
       </c>
     </row>
     <row r="2" ht="17.25" customHeight="1">

</xml_diff>

<commit_message>
il carrello non ha le ruote fissate
</commit_message>
<xml_diff>
--- a/URTI/urti_dati.xlsx
+++ b/URTI/urti_dati.xlsx
@@ -2401,7 +2401,7 @@
     <pageSetUpPr autoPageBreaks="1" fitToPage="0"/>
   </sheetPr>
   <sheetViews>
-    <sheetView topLeftCell="E1" zoomScale="100" workbookViewId="0">
+    <sheetView topLeftCell="D1" zoomScale="100" workbookViewId="0">
       <selection activeCell="A1" activeCellId="0" sqref="A1"/>
     </sheetView>
   </sheetViews>
@@ -2494,7 +2494,10 @@
         <f t="shared" ref="L2:L9" si="17">K2-J2</f>
         <v>-0.0032430000000000098</v>
       </c>
-      <c r="M2" s="29"/>
+      <c r="M2" s="29">
+        <f>(B2-C2)/C2</f>
+        <v>-0.036480686695278999</v>
+      </c>
       <c r="N2" s="11"/>
     </row>
     <row r="3" ht="17.25" customHeight="1">
@@ -2531,7 +2534,10 @@
         <f t="shared" si="17"/>
         <v>-0.0056700000000000084</v>
       </c>
-      <c r="M3" s="29"/>
+      <c r="M3" s="29">
+        <f>(B3-C3)/C3</f>
+        <v>-0.042553191489361736</v>
+      </c>
     </row>
     <row r="4" ht="17.25" customHeight="1">
       <c r="B4" s="8">
@@ -2567,7 +2573,10 @@
         <f t="shared" si="17"/>
         <v>-0.004608000000000001</v>
       </c>
-      <c r="M4" s="29"/>
+      <c r="M4" s="29">
+        <f>(B4-C4)/C4</f>
+        <v>-0.03703703703703707</v>
+      </c>
     </row>
     <row r="5" ht="17.25" customHeight="1">
       <c r="B5" s="8">
@@ -2603,7 +2612,10 @@
         <f t="shared" si="17"/>
         <v>-0.0047699999999999965</v>
       </c>
-      <c r="M5" s="29"/>
+      <c r="M5" s="29">
+        <f>(B5-C5)/C5</f>
+        <v>-0.040404040404040442</v>
+      </c>
     </row>
     <row r="6" ht="17.25" customHeight="1">
       <c r="B6" s="8">
@@ -2639,7 +2651,10 @@
         <f t="shared" si="17"/>
         <v>-0.0039060000000000206</v>
       </c>
-      <c r="M6" s="29"/>
+      <c r="M6" s="29">
+        <f>(B6-C6)/C6</f>
+        <v>-0.034482758620689689</v>
+      </c>
     </row>
     <row r="7" ht="17.25" customHeight="1">
       <c r="B7" s="8">
@@ -2675,7 +2690,10 @@
         <f t="shared" si="17"/>
         <v>-0.0051329999999999709</v>
       </c>
-      <c r="M7" s="29"/>
+      <c r="M7" s="29">
+        <f>(B7-C7)/C7</f>
+        <v>-0.033452807646355935</v>
+      </c>
     </row>
     <row r="8" ht="17.25" customHeight="1">
       <c r="B8" s="8">
@@ -2711,7 +2729,10 @@
         <f t="shared" si="17"/>
         <v>-0.0014610000000000178</v>
       </c>
-      <c r="M8" s="29"/>
+      <c r="M8" s="29">
+        <f>(B8-C8)/C8</f>
+        <v>-0.017084282460136688</v>
+      </c>
     </row>
     <row r="9" ht="17.25" customHeight="1">
       <c r="B9" s="8">
@@ -2747,7 +2768,10 @@
         <f t="shared" si="17"/>
         <v>-0.0055709999999999649</v>
       </c>
-      <c r="M9" s="29"/>
+      <c r="M9" s="29">
+        <f>(B9-C9)/C9</f>
+        <v>-0.04052098408104185</v>
+      </c>
     </row>
     <row r="10" ht="17.25" customHeight="1">
       <c r="B10" s="8"/>

</xml_diff>